<commit_message>
update regression data for linux
</commit_message>
<xml_diff>
--- a/tests/regression_data_linux/design_optimization_linux.xlsx
+++ b/tests/regression_data_linux/design_optimization_linux.xlsx
@@ -500,7 +500,7 @@
         <v>1585000</v>
       </c>
       <c r="F2" t="n">
-        <v>3978.880772777501</v>
+        <v>3978.168359302438</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -648,70 +648,70 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>2.227048603099185</v>
+        <v>2.227098522413201</v>
       </c>
       <c r="C2" t="n">
-        <v>2.283911792949138</v>
+        <v>2.283911926098509</v>
       </c>
       <c r="D2" t="n">
-        <v>10.65999932430811</v>
+        <v>10.65999725096994</v>
       </c>
       <c r="E2" t="n">
-        <v>93.79674136772066</v>
+        <v>93.79444625187517</v>
       </c>
       <c r="F2" t="n">
-        <v>90.95588592855573</v>
+        <v>90.95617585575954</v>
       </c>
       <c r="G2" t="n">
-        <v>0.03028735751093587</v>
+        <v>0.03026053790534423</v>
       </c>
       <c r="H2" t="n">
-        <v>-89.98617328606666</v>
+        <v>-89.98643639366489</v>
       </c>
       <c r="I2" t="n">
-        <v>227361.1051920489</v>
+        <v>227361.7856976638</v>
       </c>
       <c r="J2" t="n">
-        <v>57.14197488590165</v>
+        <v>57.15237897511484</v>
       </c>
       <c r="K2" t="n">
-        <v>3978.880772777501</v>
+        <v>3978.168359302438</v>
       </c>
       <c r="L2" t="n">
-        <v>2.537794679040104</v>
+        <v>2.447865779778642</v>
       </c>
       <c r="M2" t="n">
-        <v>37.68858070749693</v>
+        <v>37.67189029906209</v>
       </c>
       <c r="N2" t="n">
         <v>216.5604229337033</v>
       </c>
       <c r="O2" t="n">
-        <v>185.7797396241413</v>
+        <v>185.7727854477948</v>
       </c>
       <c r="P2" t="n">
-        <v>0.8578656113957398</v>
+        <v>0.8578334994509423</v>
       </c>
       <c r="Q2" t="n">
         <v>497686.3106529794</v>
       </c>
       <c r="R2" t="n">
-        <v>476357.8754181295</v>
+        <v>476357.8074324953</v>
       </c>
       <c r="S2" t="n">
         <v>474237.1022624383</v>
       </c>
       <c r="T2" t="n">
-        <v>0.9118683946374639</v>
+        <v>0.9117050371144925</v>
       </c>
       <c r="U2" t="n">
-        <v>0.7003745741540444</v>
+        <v>0.7003337366104763</v>
       </c>
       <c r="V2" t="n">
-        <v>0.8578656113957398</v>
+        <v>0.8578334994509423</v>
       </c>
       <c r="W2" t="n">
-        <v>1.015356648637435</v>
+        <v>1.015333262291408</v>
       </c>
     </row>
   </sheetData>
@@ -1408,10 +1408,10 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>12.36813180100213</v>
+        <v>12.36461153781507</v>
       </c>
       <c r="D2" t="n">
-        <v>12.36813180100213</v>
+        <v>12.36461153781507</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -1420,10 +1420,10 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>12.36813180100213</v>
+        <v>12.36461153781507</v>
       </c>
       <c r="H2" t="n">
-        <v>12.36813180100213</v>
+        <v>12.36461153781507</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -1432,102 +1432,102 @@
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>463.0424938037678</v>
+        <v>463.0425549789936</v>
       </c>
       <c r="L2" t="n">
-        <v>3610362.320760651</v>
+        <v>3610367.799084014</v>
       </c>
       <c r="M2" t="n">
-        <v>125.8427999914099</v>
+        <v>125.8429866097443</v>
       </c>
       <c r="N2" t="n">
-        <v>468920.3625763534</v>
+        <v>468920.405121267</v>
       </c>
       <c r="O2" t="n">
-        <v>497609.8253108689</v>
+        <v>497609.8688438679</v>
       </c>
       <c r="P2" t="n">
-        <v>1837.707528152813</v>
+        <v>1837.707528152731</v>
       </c>
       <c r="Q2" t="n">
-        <v>-353326.8514069674</v>
+        <v>-353326.9202961038</v>
       </c>
       <c r="R2" t="n">
-        <v>962.2109933110439</v>
+        <v>962.2110801832656</v>
       </c>
       <c r="S2" t="n">
-        <v>1093.998135398201</v>
+        <v>1093.998310804228</v>
       </c>
       <c r="T2" t="n">
-        <v>1.136962831440604</v>
+        <v>1.136962911085852</v>
       </c>
       <c r="U2" t="n">
-        <v>0.8943872101361351</v>
+        <v>0.8943871227767994</v>
       </c>
       <c r="V2" t="n">
-        <v>171.33523723482</v>
+        <v>171.3352404217408</v>
       </c>
       <c r="W2" t="n">
-        <v>3694211.47703007</v>
+        <v>3694217.092782319</v>
       </c>
       <c r="X2" t="n">
-        <v>2.706937613663475e-07</v>
+        <v>2.706933498720956e-07</v>
       </c>
       <c r="Y2" t="n">
-        <v>3249192.827481675</v>
+        <v>3249197.539130076</v>
       </c>
       <c r="Z2" t="n">
-        <v>3.077687453763898e-07</v>
+        <v>3.077682990821589e-07</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.003320110508457271</v>
+        <v>0.003320111458885236</v>
       </c>
       <c r="AB2" t="n">
-        <v>2.133802362966454e-05</v>
+        <v>2.133803001401621e-05</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.02951135828691635</v>
+        <v>0.02951136730659603</v>
       </c>
       <c r="AD2" t="n">
-        <v>16.2833947310557</v>
+        <v>16.28785921211356</v>
       </c>
       <c r="AE2" t="inlineStr"/>
       <c r="AF2" t="inlineStr"/>
       <c r="AG2" t="n">
-        <v>3610362.320760651</v>
+        <v>3610367.799084014</v>
       </c>
       <c r="AH2" t="n">
-        <v>125.8427999914099</v>
+        <v>125.8429866097443</v>
       </c>
       <c r="AI2" t="n">
-        <v>125.8427999914099</v>
+        <v>125.8429866097443</v>
       </c>
       <c r="AJ2" t="n">
-        <v>468920.3625763534</v>
+        <v>468920.405121267</v>
       </c>
       <c r="AK2" t="n">
-        <v>497609.8253108689</v>
+        <v>497609.8688438679</v>
       </c>
       <c r="AL2" t="n">
-        <v>1837.707528152813</v>
+        <v>1837.707528152731</v>
       </c>
       <c r="AM2" t="n">
-        <v>962.2109933110439</v>
+        <v>962.2110801832656</v>
       </c>
       <c r="AN2" t="n">
-        <v>1093.998135398201</v>
+        <v>1093.998310804228</v>
       </c>
       <c r="AO2" t="n">
-        <v>171.33523723482</v>
+        <v>171.3352404217408</v>
       </c>
       <c r="AP2" t="n">
-        <v>0.8943872101361351</v>
+        <v>0.8943871227767994</v>
       </c>
       <c r="AQ2" t="n">
-        <v>2.133802362966454e-05</v>
+        <v>2.133803001401621e-05</v>
       </c>
       <c r="AR2" t="n">
-        <v>0.02951135828691635</v>
+        <v>0.02951136730659603</v>
       </c>
       <c r="AS2" t="inlineStr">
         <is>
@@ -1753,16 +1753,16 @@
       </c>
       <c r="DQ2" t="inlineStr"/>
       <c r="DR2" t="n">
-        <v>0.07218673753637289</v>
+        <v>0.07216619013916603</v>
       </c>
       <c r="DS2" t="n">
-        <v>0.07218673753637289</v>
+        <v>0.07216619013916603</v>
       </c>
       <c r="DT2" t="n">
-        <v>756605.4693984861</v>
+        <v>757377.4893452935</v>
       </c>
       <c r="DU2" t="n">
-        <v>10.65999984611691</v>
+        <v>10.6600007212342</v>
       </c>
       <c r="DV2" t="n">
         <v>497686.3106530505</v>
@@ -1816,126 +1816,126 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>118.6452749957528</v>
+        <v>118.5890409160816</v>
       </c>
       <c r="D3" t="n">
-        <v>22.59573697776639</v>
+        <v>22.58473243477841</v>
       </c>
       <c r="E3" t="n">
-        <v>116.4737478973241</v>
+        <v>116.4186002589172</v>
       </c>
       <c r="F3" t="n">
-        <v>79.02107891490891</v>
+        <v>79.02122404287434</v>
       </c>
       <c r="G3" t="n">
-        <v>118.6452749957528</v>
+        <v>118.5890409160816</v>
       </c>
       <c r="H3" t="n">
-        <v>22.59573697776639</v>
+        <v>22.58473243477841</v>
       </c>
       <c r="I3" t="n">
-        <v>116.4737478973241</v>
+        <v>116.4186002589172</v>
       </c>
       <c r="J3" t="n">
-        <v>79.02107891490891</v>
+        <v>79.02122404287434</v>
       </c>
       <c r="K3" t="n">
-        <v>453.2704351765942</v>
+        <v>453.2795543839204</v>
       </c>
       <c r="L3" t="n">
-        <v>2786607.121814948</v>
+        <v>2787292.872697627</v>
       </c>
       <c r="M3" t="n">
-        <v>97.58767334008263</v>
+        <v>97.61119793809797</v>
       </c>
       <c r="N3" t="n">
-        <v>462093.0511153506</v>
+        <v>462099.5779327312</v>
       </c>
       <c r="O3" t="n">
-        <v>490647.9600135669</v>
+        <v>490654.630340399</v>
       </c>
       <c r="P3" t="n">
-        <v>1838.692343556171</v>
+        <v>1838.691558492078</v>
       </c>
       <c r="Q3" t="n">
-        <v>-342776.9187060104</v>
+        <v>-342786.6599423661</v>
       </c>
       <c r="R3" t="n">
-        <v>948.0589154758175</v>
+        <v>948.0721186970139</v>
       </c>
       <c r="S3" t="n">
-        <v>1066.244692553487</v>
+        <v>1066.269220306893</v>
       </c>
       <c r="T3" t="n">
-        <v>1.124660793911056</v>
+        <v>1.124671002636723</v>
       </c>
       <c r="U3" t="n">
-        <v>0.9093841893915031</v>
+        <v>0.909370464374556</v>
       </c>
       <c r="V3" t="n">
-        <v>171.1100718092394</v>
+        <v>171.1101913520741</v>
       </c>
       <c r="W3" t="n">
-        <v>2857235.98339369</v>
+        <v>2857928.745294577</v>
       </c>
       <c r="X3" t="n">
-        <v>3.499885924060943e-07</v>
+        <v>3.499037551745982e-07</v>
       </c>
       <c r="Y3" t="n">
-        <v>2540531.330746874</v>
+        <v>2541124.238638977</v>
       </c>
       <c r="Z3" t="n">
-        <v>3.936184481952508e-07</v>
+        <v>3.935266071585696e-07</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.003164747863918395</v>
+        <v>0.003164879799521958</v>
       </c>
       <c r="AB3" t="n">
-        <v>2.039198697008735e-05</v>
+        <v>2.039277866940487e-05</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.02811848711078169</v>
+        <v>0.02811971843373368</v>
       </c>
       <c r="AD3" t="n">
-        <v>3.146596678903728</v>
+        <v>3.147527009748639</v>
       </c>
       <c r="AE3" t="inlineStr"/>
       <c r="AF3" t="inlineStr"/>
       <c r="AG3" t="n">
-        <v>2786607.121814948</v>
+        <v>2787292.872697627</v>
       </c>
       <c r="AH3" t="n">
-        <v>97.58767334008263</v>
+        <v>97.61119793809797</v>
       </c>
       <c r="AI3" t="n">
-        <v>97.58767334008263</v>
+        <v>97.61119793809797</v>
       </c>
       <c r="AJ3" t="n">
-        <v>462093.0511153506</v>
+        <v>462099.5779327312</v>
       </c>
       <c r="AK3" t="n">
-        <v>490647.9600135669</v>
+        <v>490654.630340399</v>
       </c>
       <c r="AL3" t="n">
-        <v>1838.692343556171</v>
+        <v>1838.691558492078</v>
       </c>
       <c r="AM3" t="n">
-        <v>948.0589154758175</v>
+        <v>948.0721186970139</v>
       </c>
       <c r="AN3" t="n">
-        <v>1066.244692553487</v>
+        <v>1066.269220306893</v>
       </c>
       <c r="AO3" t="n">
-        <v>171.1100718092394</v>
+        <v>171.1101913520741</v>
       </c>
       <c r="AP3" t="n">
-        <v>0.9093841893915031</v>
+        <v>0.909370464374556</v>
       </c>
       <c r="AQ3" t="n">
-        <v>2.039198697008735e-05</v>
+        <v>2.039277866940487e-05</v>
       </c>
       <c r="AR3" t="n">
-        <v>0.02811848711078169</v>
+        <v>0.02811971843373368</v>
       </c>
       <c r="AS3" t="inlineStr">
         <is>
@@ -1947,102 +1947,102 @@
       </c>
       <c r="AU3" t="inlineStr"/>
       <c r="AV3" t="n">
-        <v>462.9273048079153</v>
+        <v>462.9274809464312</v>
       </c>
       <c r="AW3" t="n">
-        <v>3562948.754173271</v>
+        <v>3562993.839886291</v>
       </c>
       <c r="AX3" t="n">
-        <v>124.0561232970211</v>
+        <v>124.057793479354</v>
       </c>
       <c r="AY3" t="n">
-        <v>468965.8520455072</v>
+        <v>468965.8752820299</v>
       </c>
       <c r="AZ3" t="n">
-        <v>497686.3106531221</v>
+        <v>497686.3106529787</v>
       </c>
       <c r="BA3" t="n">
-        <v>1838.692343556171</v>
+        <v>1838.691558492096</v>
       </c>
       <c r="BB3" t="n">
-        <v>-353494.5803202856</v>
+        <v>-353494.540757235</v>
       </c>
       <c r="BC3" t="n">
-        <v>961.8197746113447</v>
+        <v>961.8202053177442</v>
       </c>
       <c r="BD3" t="n">
-        <v>1092.587192209621</v>
+        <v>1092.588550031381</v>
       </c>
       <c r="BE3" t="n">
-        <v>1.135958337570173</v>
+        <v>1.135959240605095</v>
       </c>
       <c r="BF3" t="n">
-        <v>0.8955762876232903</v>
+        <v>0.8955752222893982</v>
       </c>
       <c r="BG3" t="n">
-        <v>171.4468311442109</v>
+        <v>171.4467463557218</v>
       </c>
       <c r="BH3" t="n">
-        <v>3646507.661850082</v>
+        <v>3646553.148430774</v>
       </c>
       <c r="BI3" t="n">
-        <v>2.742349921438648e-07</v>
+        <v>2.742315713759256e-07</v>
       </c>
       <c r="BJ3" t="n">
-        <v>3210071.656016892</v>
+        <v>3210109.14659962</v>
       </c>
       <c r="BK3" t="n">
-        <v>3.115195257793142e-07</v>
+        <v>3.115158875701384e-07</v>
       </c>
       <c r="BL3" t="n">
-        <v>0.003304038613814681</v>
+        <v>0.003304052645003351</v>
       </c>
       <c r="BM3" t="n">
-        <v>2.129511500268102e-05</v>
+        <v>2.129515759501139e-05</v>
       </c>
       <c r="BN3" t="n">
-        <v>0.02946792321494149</v>
+        <v>0.02946796998673389</v>
       </c>
       <c r="BO3" t="n">
-        <v>8.028441337682555</v>
+        <v>8.030676119275515</v>
       </c>
       <c r="BP3" t="inlineStr"/>
       <c r="BQ3" t="inlineStr"/>
       <c r="BR3" t="n">
-        <v>3562948.754173271</v>
+        <v>3562993.839886291</v>
       </c>
       <c r="BS3" t="n">
-        <v>124.0561232970211</v>
+        <v>124.057793479354</v>
       </c>
       <c r="BT3" t="n">
-        <v>124.0561232970211</v>
+        <v>124.057793479354</v>
       </c>
       <c r="BU3" t="n">
-        <v>468965.8520455072</v>
+        <v>468965.8752820299</v>
       </c>
       <c r="BV3" t="n">
-        <v>497686.3106531221</v>
+        <v>497686.3106529787</v>
       </c>
       <c r="BW3" t="n">
-        <v>1838.692343556171</v>
+        <v>1838.691558492096</v>
       </c>
       <c r="BX3" t="n">
-        <v>961.8197746113447</v>
+        <v>961.8202053177442</v>
       </c>
       <c r="BY3" t="n">
-        <v>1092.587192209621</v>
+        <v>1092.588550031381</v>
       </c>
       <c r="BZ3" t="n">
-        <v>171.4468311442109</v>
+        <v>171.4467463557218</v>
       </c>
       <c r="CA3" t="n">
-        <v>0.8955762876232903</v>
+        <v>0.8955752222893982</v>
       </c>
       <c r="CB3" t="n">
-        <v>2.129511500268102e-05</v>
+        <v>2.129515759501139e-05</v>
       </c>
       <c r="CC3" t="n">
-        <v>0.02946792321494149</v>
+        <v>0.02946796998673389</v>
       </c>
       <c r="CD3" t="inlineStr">
         <is>
@@ -2054,102 +2054,102 @@
       </c>
       <c r="CF3" t="inlineStr"/>
       <c r="CG3" t="n">
-        <v>462.9273048079153</v>
+        <v>462.9274809464312</v>
       </c>
       <c r="CH3" t="n">
-        <v>3562948.754173271</v>
+        <v>3562993.839886291</v>
       </c>
       <c r="CI3" t="n">
-        <v>124.0561232970211</v>
+        <v>124.057793479354</v>
       </c>
       <c r="CJ3" t="n">
-        <v>468965.8520455072</v>
+        <v>468965.8752820299</v>
       </c>
       <c r="CK3" t="n">
-        <v>497686.3106531221</v>
+        <v>497686.3106529787</v>
       </c>
       <c r="CL3" t="n">
-        <v>1838.692343556171</v>
+        <v>1838.691558492096</v>
       </c>
       <c r="CM3" t="n">
-        <v>-353494.5803202856</v>
+        <v>-353494.540757235</v>
       </c>
       <c r="CN3" t="n">
-        <v>961.8197746113447</v>
+        <v>961.8202053177442</v>
       </c>
       <c r="CO3" t="n">
-        <v>1092.587192209621</v>
+        <v>1092.588550031381</v>
       </c>
       <c r="CP3" t="n">
-        <v>1.135958337570173</v>
+        <v>1.135959240605095</v>
       </c>
       <c r="CQ3" t="n">
-        <v>0.8955762876232903</v>
+        <v>0.8955752222893982</v>
       </c>
       <c r="CR3" t="n">
-        <v>171.4468311442109</v>
+        <v>171.4467463557218</v>
       </c>
       <c r="CS3" t="n">
-        <v>3646507.661850082</v>
+        <v>3646553.148430774</v>
       </c>
       <c r="CT3" t="n">
-        <v>2.742349921438648e-07</v>
+        <v>2.742315713759256e-07</v>
       </c>
       <c r="CU3" t="n">
-        <v>3210071.656016892</v>
+        <v>3210109.14659962</v>
       </c>
       <c r="CV3" t="n">
-        <v>3.115195257793142e-07</v>
+        <v>3.115158875701384e-07</v>
       </c>
       <c r="CW3" t="n">
-        <v>0.003304038613814681</v>
+        <v>0.003304052645003351</v>
       </c>
       <c r="CX3" t="n">
-        <v>2.129511500268102e-05</v>
+        <v>2.129515759501139e-05</v>
       </c>
       <c r="CY3" t="n">
-        <v>0.02946792321494149</v>
+        <v>0.02946796998673389</v>
       </c>
       <c r="CZ3" t="n">
-        <v>8.028441337682555</v>
+        <v>8.030676119275515</v>
       </c>
       <c r="DA3" t="inlineStr"/>
       <c r="DB3" t="inlineStr"/>
       <c r="DC3" t="n">
-        <v>3562948.754173271</v>
+        <v>3562993.839886291</v>
       </c>
       <c r="DD3" t="n">
-        <v>124.0561232970211</v>
+        <v>124.057793479354</v>
       </c>
       <c r="DE3" t="n">
-        <v>124.0561232970211</v>
+        <v>124.057793479354</v>
       </c>
       <c r="DF3" t="n">
-        <v>468965.8520455072</v>
+        <v>468965.8752820299</v>
       </c>
       <c r="DG3" t="n">
-        <v>497686.3106531221</v>
+        <v>497686.3106529787</v>
       </c>
       <c r="DH3" t="n">
-        <v>1838.692343556171</v>
+        <v>1838.691558492096</v>
       </c>
       <c r="DI3" t="n">
-        <v>961.8197746113447</v>
+        <v>961.8202053177442</v>
       </c>
       <c r="DJ3" t="n">
-        <v>1092.587192209621</v>
+        <v>1092.588550031381</v>
       </c>
       <c r="DK3" t="n">
-        <v>171.4468311442109</v>
+        <v>171.4467463557218</v>
       </c>
       <c r="DL3" t="n">
-        <v>0.8955762876232903</v>
+        <v>0.8955752222893982</v>
       </c>
       <c r="DM3" t="n">
-        <v>2.129511500268102e-05</v>
+        <v>2.129515759501139e-05</v>
       </c>
       <c r="DN3" t="n">
-        <v>0.02946792321494149</v>
+        <v>0.02946796998673389</v>
       </c>
       <c r="DO3" t="inlineStr">
         <is>
@@ -2161,40 +2161,40 @@
       </c>
       <c r="DQ3" t="inlineStr"/>
       <c r="DR3" t="n">
-        <v>0.6933856887630991</v>
+        <v>0.6930565618506871</v>
       </c>
       <c r="DS3" t="n">
-        <v>0.6933856887630991</v>
+        <v>0.6930565618506871</v>
       </c>
       <c r="DT3" t="n">
-        <v>5889481.431522566</v>
+        <v>5895559.340410924</v>
       </c>
       <c r="DU3" t="n">
-        <v>10.65999966522349</v>
+        <v>10.65999922076366</v>
       </c>
       <c r="DV3" t="n">
         <v>497686.3106530505</v>
       </c>
       <c r="DW3" t="n">
-        <v>0.01980130068621652</v>
+        <v>0.01979882120425101</v>
       </c>
       <c r="DX3" t="n">
         <v>0</v>
       </c>
       <c r="DY3" t="n">
-        <v>0.01172129159082114</v>
+        <v>0.01172092194423158</v>
       </c>
       <c r="DZ3" t="n">
-        <v>0.04196859139198431</v>
+        <v>0.04197016482468759</v>
       </c>
       <c r="EA3" t="n">
         <v>0</v>
       </c>
       <c r="EB3" t="n">
-        <v>0.07349118366902196</v>
+        <v>0.07348990797317018</v>
       </c>
       <c r="EC3" t="n">
-        <v>-3.889674760115813e-06</v>
+        <v>-4.204655697226389e-08</v>
       </c>
       <c r="ED3" t="n">
         <v>0</v>
@@ -2205,129 +2205,129 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>185.7797396241413</v>
+        <v>185.7727854477948</v>
       </c>
       <c r="C4" t="n">
-        <v>118.6452749957675</v>
+        <v>118.5890409160617</v>
       </c>
       <c r="D4" t="n">
-        <v>22.59573697784346</v>
+        <v>22.58473243467366</v>
       </c>
       <c r="E4" t="n">
-        <v>116.4737478973241</v>
+        <v>116.4186002589172</v>
       </c>
       <c r="F4" t="n">
-        <v>79.02107891487238</v>
+        <v>79.02122404292402</v>
       </c>
       <c r="G4" t="n">
-        <v>72.89641842237207</v>
+        <v>72.93883151215769</v>
       </c>
       <c r="H4" t="n">
-        <v>22.59573697784346</v>
+        <v>22.58473243467366</v>
       </c>
       <c r="I4" t="n">
-        <v>-69.30599172681727</v>
+        <v>-69.35418518887759</v>
       </c>
       <c r="J4" t="n">
-        <v>-71.94254919870754</v>
+        <v>-71.96250255596031</v>
       </c>
       <c r="K4" t="n">
-        <v>453.2704351767158</v>
+        <v>453.2795543837262</v>
       </c>
       <c r="L4" t="n">
-        <v>2786607.12181159</v>
+        <v>2787292.872693905</v>
       </c>
       <c r="M4" t="n">
-        <v>97.58767333991611</v>
+        <v>97.61119793801501</v>
       </c>
       <c r="N4" t="n">
-        <v>462093.0511154808</v>
+        <v>462099.5779325545</v>
       </c>
       <c r="O4" t="n">
-        <v>490647.9600137114</v>
+        <v>490654.6303402084</v>
       </c>
       <c r="P4" t="n">
-        <v>1838.692343556565</v>
+        <v>1838.691558491741</v>
       </c>
       <c r="Q4" t="n">
-        <v>-342776.9187062682</v>
+        <v>-342786.659942047</v>
       </c>
       <c r="R4" t="n">
-        <v>948.0589154759082</v>
+        <v>948.0721186968073</v>
       </c>
       <c r="S4" t="n">
-        <v>1066.244692553445</v>
+        <v>1066.269220306692</v>
       </c>
       <c r="T4" t="n">
-        <v>1.124660793910903</v>
+        <v>1.124671002636756</v>
       </c>
       <c r="U4" t="n">
-        <v>0.9093841893917152</v>
+        <v>0.9093704643745042</v>
       </c>
       <c r="V4" t="n">
-        <v>171.1100718092908</v>
+        <v>171.1101913520281</v>
       </c>
       <c r="W4" t="n">
-        <v>2857235.983390532</v>
+        <v>2857928.745290611</v>
       </c>
       <c r="X4" t="n">
-        <v>3.499885924064811e-07</v>
+        <v>3.499037551750836e-07</v>
       </c>
       <c r="Y4" t="n">
-        <v>2540531.33074441</v>
+        <v>2541124.238635376</v>
       </c>
       <c r="Z4" t="n">
-        <v>3.936184481956325e-07</v>
+        <v>3.935266071591273e-07</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.003164747863915027</v>
+        <v>0.003164879799523613</v>
       </c>
       <c r="AB4" t="n">
-        <v>2.039198697008857e-05</v>
+        <v>2.039277866939614e-05</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.02811848711078983</v>
+        <v>0.02811971843371466</v>
       </c>
       <c r="AD4" t="n">
-        <v>3.146596678901791</v>
+        <v>3.147527009741291</v>
       </c>
       <c r="AE4" t="inlineStr"/>
       <c r="AF4" t="inlineStr"/>
       <c r="AG4" t="n">
-        <v>2786607.12181159</v>
+        <v>2787292.872693905</v>
       </c>
       <c r="AH4" t="n">
-        <v>97.58767333991611</v>
+        <v>97.61119793801501</v>
       </c>
       <c r="AI4" t="n">
-        <v>97.58767333991611</v>
+        <v>97.61119793801501</v>
       </c>
       <c r="AJ4" t="n">
-        <v>462093.0511154808</v>
+        <v>462099.5779325545</v>
       </c>
       <c r="AK4" t="n">
-        <v>490647.9600137114</v>
+        <v>490654.6303402084</v>
       </c>
       <c r="AL4" t="n">
-        <v>1838.692343556565</v>
+        <v>1838.691558491741</v>
       </c>
       <c r="AM4" t="n">
-        <v>948.0589154759082</v>
+        <v>948.0721186968073</v>
       </c>
       <c r="AN4" t="n">
-        <v>1066.244692553445</v>
+        <v>1066.269220306692</v>
       </c>
       <c r="AO4" t="n">
-        <v>171.1100718092908</v>
+        <v>171.1101913520281</v>
       </c>
       <c r="AP4" t="n">
-        <v>0.9093841893917152</v>
+        <v>0.9093704643745042</v>
       </c>
       <c r="AQ4" t="n">
-        <v>2.039198697008857e-05</v>
+        <v>2.039277866939614e-05</v>
       </c>
       <c r="AR4" t="n">
-        <v>0.02811848711078983</v>
+        <v>0.02811971843371466</v>
       </c>
       <c r="AS4" t="inlineStr">
         <is>
@@ -2339,102 +2339,102 @@
       </c>
       <c r="AU4" t="inlineStr"/>
       <c r="AV4" t="n">
-        <v>462.9273048077678</v>
+        <v>462.9274809464064</v>
       </c>
       <c r="AW4" t="n">
-        <v>3562948.754146125</v>
+        <v>3562993.839890544</v>
       </c>
       <c r="AX4" t="n">
-        <v>124.0561232960325</v>
+        <v>124.0577934795285</v>
       </c>
       <c r="AY4" t="n">
-        <v>468965.852045452</v>
+        <v>468965.8752819909</v>
       </c>
       <c r="AZ4" t="n">
-        <v>497686.310653077</v>
+        <v>497686.3106529335</v>
       </c>
       <c r="BA4" t="n">
-        <v>1838.692343556546</v>
+        <v>1838.691558491925</v>
       </c>
       <c r="BB4" t="n">
-        <v>-353494.5803202333</v>
+        <v>-353494.5407571552</v>
       </c>
       <c r="BC4" t="n">
-        <v>961.8197746110494</v>
+        <v>961.8202053177483</v>
       </c>
       <c r="BD4" t="n">
-        <v>1092.587192208793</v>
+        <v>1092.588550031498</v>
       </c>
       <c r="BE4" t="n">
-        <v>1.13595833756966</v>
+        <v>1.135959240605211</v>
       </c>
       <c r="BF4" t="n">
-        <v>0.8955762876238892</v>
+        <v>0.8955752222892553</v>
       </c>
       <c r="BG4" t="n">
-        <v>171.4468311442482</v>
+        <v>171.4467463557</v>
       </c>
       <c r="BH4" t="n">
-        <v>3646507.661822607</v>
+        <v>3646553.148434978</v>
       </c>
       <c r="BI4" t="n">
-        <v>2.742349921459311e-07</v>
+        <v>2.742315713756095e-07</v>
       </c>
       <c r="BJ4" t="n">
-        <v>3210071.655994155</v>
+        <v>3210109.146602992</v>
       </c>
       <c r="BK4" t="n">
-        <v>3.115195257815207e-07</v>
+        <v>3.115158875698112e-07</v>
       </c>
       <c r="BL4" t="n">
-        <v>0.00330403861380701</v>
+        <v>0.003304052645005448</v>
       </c>
       <c r="BM4" t="n">
-        <v>2.129511500265488e-05</v>
+        <v>2.129515759501463e-05</v>
       </c>
       <c r="BN4" t="n">
-        <v>0.02946792321490987</v>
+        <v>0.02946796998673484</v>
       </c>
       <c r="BO4" t="n">
-        <v>8.028441336334996</v>
+        <v>8.030676119479546</v>
       </c>
       <c r="BP4" t="inlineStr"/>
       <c r="BQ4" t="inlineStr"/>
       <c r="BR4" t="n">
-        <v>3562948.754146125</v>
+        <v>3562993.839890544</v>
       </c>
       <c r="BS4" t="n">
-        <v>124.0561232960325</v>
+        <v>124.0577934795285</v>
       </c>
       <c r="BT4" t="n">
-        <v>124.0561232960325</v>
+        <v>124.0577934795285</v>
       </c>
       <c r="BU4" t="n">
-        <v>468965.852045452</v>
+        <v>468965.8752819909</v>
       </c>
       <c r="BV4" t="n">
-        <v>497686.310653077</v>
+        <v>497686.3106529335</v>
       </c>
       <c r="BW4" t="n">
-        <v>1838.692343556546</v>
+        <v>1838.691558491925</v>
       </c>
       <c r="BX4" t="n">
-        <v>961.8197746110494</v>
+        <v>961.8202053177483</v>
       </c>
       <c r="BY4" t="n">
-        <v>1092.587192208793</v>
+        <v>1092.588550031498</v>
       </c>
       <c r="BZ4" t="n">
-        <v>171.4468311442482</v>
+        <v>171.4467463557</v>
       </c>
       <c r="CA4" t="n">
-        <v>0.8955762876238892</v>
+        <v>0.8955752222892553</v>
       </c>
       <c r="CB4" t="n">
-        <v>2.129511500265488e-05</v>
+        <v>2.129515759501463e-05</v>
       </c>
       <c r="CC4" t="n">
-        <v>0.02946792321490987</v>
+        <v>0.02946796998673484</v>
       </c>
       <c r="CD4" t="inlineStr">
         <is>
@@ -2446,102 +2446,102 @@
       </c>
       <c r="CF4" t="inlineStr"/>
       <c r="CG4" t="n">
-        <v>456.8709521301843</v>
+        <v>456.8844361504757</v>
       </c>
       <c r="CH4" t="n">
-        <v>3058016.392946888</v>
+        <v>3059098.105270364</v>
       </c>
       <c r="CI4" t="n">
-        <v>106.8524588379397</v>
+        <v>106.8894769712893</v>
       </c>
       <c r="CJ4" t="n">
-        <v>464685.8489552091</v>
+        <v>464695.4034260194</v>
       </c>
       <c r="CK4" t="n">
-        <v>493304.9039231897</v>
+        <v>493314.6669115357</v>
       </c>
       <c r="CL4" t="n">
-        <v>1838.692343556557</v>
+        <v>1838.691558491936</v>
       </c>
       <c r="CM4" t="n">
-        <v>-346740.2177519748</v>
+        <v>-346754.8890446919</v>
       </c>
       <c r="CN4" t="n">
-        <v>953.2015318365337</v>
+        <v>953.2209413461285</v>
       </c>
       <c r="CO4" t="n">
-        <v>1075.801501575445</v>
+        <v>1075.838647067924</v>
       </c>
       <c r="CP4" t="n">
-        <v>1.128619148883131</v>
+        <v>1.128635136308101</v>
       </c>
       <c r="CQ4" t="n">
-        <v>0.9042442494174991</v>
+        <v>0.9042241505776647</v>
       </c>
       <c r="CR4" t="n">
-        <v>171.2068484868605</v>
+        <v>171.2071648474618</v>
       </c>
       <c r="CS4" t="n">
-        <v>3132036.29684554</v>
+        <v>3133132.943352118</v>
       </c>
       <c r="CT4" t="n">
-        <v>3.192811018847896e-07</v>
+        <v>3.191693484062973e-07</v>
       </c>
       <c r="CU4" t="n">
-        <v>2775104.693150892</v>
+        <v>2776037.040279435</v>
       </c>
       <c r="CV4" t="n">
-        <v>3.603467654636792e-07</v>
+        <v>3.602257410439092e-07</v>
       </c>
       <c r="CW4" t="n">
-        <v>0.003214407868482763</v>
+        <v>0.003214609757833506</v>
       </c>
       <c r="CX4" t="n">
-        <v>2.070850682739516e-05</v>
+        <v>2.070975438012401e-05</v>
       </c>
       <c r="CY4" t="n">
-        <v>0.02860670421702007</v>
+        <v>0.02860858259689537</v>
       </c>
       <c r="CZ4" t="n">
-        <v>3.62271164400715</v>
+        <v>3.625180120705648</v>
       </c>
       <c r="DA4" t="inlineStr"/>
       <c r="DB4" t="inlineStr"/>
       <c r="DC4" t="n">
-        <v>3058016.392946888</v>
+        <v>3059098.105270364</v>
       </c>
       <c r="DD4" t="n">
-        <v>106.8524588379397</v>
+        <v>106.8894769712893</v>
       </c>
       <c r="DE4" t="n">
-        <v>106.8524588379397</v>
+        <v>106.8894769712893</v>
       </c>
       <c r="DF4" t="n">
-        <v>464685.8489552091</v>
+        <v>464695.4034260194</v>
       </c>
       <c r="DG4" t="n">
-        <v>493304.9039231897</v>
+        <v>493314.6669115357</v>
       </c>
       <c r="DH4" t="n">
-        <v>1838.692343556557</v>
+        <v>1838.691558491936</v>
       </c>
       <c r="DI4" t="n">
-        <v>953.2015318365337</v>
+        <v>953.2209413461285</v>
       </c>
       <c r="DJ4" t="n">
-        <v>1075.801501575445</v>
+        <v>1075.838647067924</v>
       </c>
       <c r="DK4" t="n">
-        <v>171.2068484868605</v>
+        <v>171.2071648474618</v>
       </c>
       <c r="DL4" t="n">
-        <v>0.9042442494174991</v>
+        <v>0.9042241505776647</v>
       </c>
       <c r="DM4" t="n">
-        <v>2.070850682739516e-05</v>
+        <v>2.070975438012401e-05</v>
       </c>
       <c r="DN4" t="n">
-        <v>0.02860670421702007</v>
+        <v>0.02860858259689537</v>
       </c>
       <c r="DO4" t="inlineStr">
         <is>
@@ -2553,19 +2553,19 @@
       </c>
       <c r="DQ4" t="inlineStr"/>
       <c r="DR4" t="n">
-        <v>0.6933856887629765</v>
+        <v>0.6930565618507568</v>
       </c>
       <c r="DS4" t="n">
-        <v>0.4260206173229715</v>
+        <v>0.4262681897310215</v>
       </c>
       <c r="DT4" t="n">
-        <v>2932296.145410848</v>
+        <v>2935096.663930992</v>
       </c>
       <c r="DU4" t="n">
-        <v>10.6599996652053</v>
+        <v>10.6599992207546</v>
       </c>
       <c r="DV4" t="n">
-        <v>476047.8480957093</v>
+        <v>476058.9030049462</v>
       </c>
       <c r="DW4" t="inlineStr"/>
       <c r="DX4" t="inlineStr"/>
@@ -2581,129 +2581,129 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>185.7797396241413</v>
+        <v>185.7727854477948</v>
       </c>
       <c r="C5" t="n">
-        <v>37.68858070749693</v>
+        <v>37.67189029906209</v>
       </c>
       <c r="D5" t="n">
-        <v>37.65161691835436</v>
+        <v>37.63751461934461</v>
       </c>
       <c r="E5" t="n">
-        <v>1.668789734808456</v>
+        <v>1.608978552743679</v>
       </c>
       <c r="F5" t="n">
-        <v>2.537794679040104</v>
+        <v>2.447865779778642</v>
       </c>
       <c r="G5" t="n">
-        <v>187.9214892600603</v>
+        <v>187.9704505415653</v>
       </c>
       <c r="H5" t="n">
-        <v>37.65161691835436</v>
+        <v>37.63751461934461</v>
       </c>
       <c r="I5" t="n">
-        <v>-184.1109498893329</v>
+        <v>-184.1638068950511</v>
       </c>
       <c r="J5" t="n">
-        <v>-78.44209189124997</v>
+        <v>-78.44953135674916</v>
       </c>
       <c r="K5" t="n">
-        <v>433.5388045266034</v>
+        <v>433.539355249771</v>
       </c>
       <c r="L5" t="n">
-        <v>1584999.91598887</v>
+        <v>1584999.823585244</v>
       </c>
       <c r="M5" t="n">
-        <v>56.29272198596961</v>
+        <v>56.29262763804503</v>
       </c>
       <c r="N5" t="n">
-        <v>447491.2694109431</v>
+        <v>447491.7847743836</v>
       </c>
       <c r="O5" t="n">
-        <v>475647.6608603371</v>
+        <v>475648.2217731432</v>
       </c>
       <c r="P5" t="n">
-        <v>1840.966337971762</v>
+        <v>1840.96763555788</v>
       </c>
       <c r="Q5" t="n">
-        <v>-322482.6844776595</v>
+        <v>-322483.6999823155</v>
       </c>
       <c r="R5" t="n">
-        <v>919.4335433151066</v>
+        <v>919.4341226073105</v>
       </c>
       <c r="S5" t="n">
-        <v>1017.696001125401</v>
+        <v>1017.696435477174</v>
       </c>
       <c r="T5" t="n">
-        <v>1.10687282242934</v>
+        <v>1.106872597452891</v>
       </c>
       <c r="U5" t="n">
-        <v>0.9375037896232532</v>
+        <v>0.9375041153398715</v>
       </c>
       <c r="V5" t="n">
-        <v>170.9238782692957</v>
+        <v>170.9240311338854</v>
       </c>
       <c r="W5" t="n">
-        <v>1644590.30577804</v>
+        <v>1644590.491058393</v>
       </c>
       <c r="X5" t="n">
-        <v>6.080541740314525e-07</v>
+        <v>6.080541055277778e-07</v>
       </c>
       <c r="Y5" t="n">
-        <v>1485798.79499483</v>
+        <v>1485799.264380459</v>
       </c>
       <c r="Z5" t="n">
-        <v>6.730386398001349e-07</v>
+        <v>6.730384271774256e-07</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.002930393532856375</v>
+        <v>0.002930386591830847</v>
       </c>
       <c r="AB5" t="n">
-        <v>1.894863437003267e-05</v>
+        <v>1.894865421349597e-05</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.02568332960893676</v>
+        <v>0.02568337701337227</v>
       </c>
       <c r="AD5" t="n">
-        <v>2.254019552939526</v>
+        <v>2.254024902798916</v>
       </c>
       <c r="AE5" t="inlineStr"/>
       <c r="AF5" t="inlineStr"/>
       <c r="AG5" t="n">
-        <v>1584999.91598887</v>
+        <v>1584999.823585244</v>
       </c>
       <c r="AH5" t="n">
-        <v>56.29272198596961</v>
+        <v>56.29262763804503</v>
       </c>
       <c r="AI5" t="n">
-        <v>56.29272198596961</v>
+        <v>56.29262763804503</v>
       </c>
       <c r="AJ5" t="n">
-        <v>447491.2694109431</v>
+        <v>447491.7847743836</v>
       </c>
       <c r="AK5" t="n">
-        <v>475647.6608603371</v>
+        <v>475648.2217731432</v>
       </c>
       <c r="AL5" t="n">
-        <v>1840.966337971762</v>
+        <v>1840.96763555788</v>
       </c>
       <c r="AM5" t="n">
-        <v>919.4335433151066</v>
+        <v>919.4341226073105</v>
       </c>
       <c r="AN5" t="n">
-        <v>1017.696001125401</v>
+        <v>1017.696435477174</v>
       </c>
       <c r="AO5" t="n">
-        <v>170.9238782692957</v>
+        <v>170.9240311338854</v>
       </c>
       <c r="AP5" t="n">
-        <v>0.9375037896232532</v>
+        <v>0.9375041153398715</v>
       </c>
       <c r="AQ5" t="n">
-        <v>1.894863437003267e-05</v>
+        <v>1.894865421349597e-05</v>
       </c>
       <c r="AR5" t="n">
-        <v>0.02568332960893676</v>
+        <v>0.02568337701337227</v>
       </c>
       <c r="AS5" t="inlineStr">
         <is>
@@ -2715,102 +2715,102 @@
       </c>
       <c r="AU5" t="inlineStr"/>
       <c r="AV5" t="n">
-        <v>434.4265374499339</v>
+        <v>434.4262997062645</v>
       </c>
       <c r="AW5" t="n">
-        <v>1625469.688857595</v>
+        <v>1625433.2547569</v>
       </c>
       <c r="AX5" t="n">
-        <v>57.67773378537485</v>
+        <v>57.67639342236885</v>
       </c>
       <c r="AY5" t="n">
-        <v>448175.9483176969</v>
+        <v>448175.8571005159</v>
       </c>
       <c r="AZ5" t="n">
-        <v>476357.8754181295</v>
+        <v>476357.8074324953</v>
       </c>
       <c r="BA5" t="n">
-        <v>1840.966337971765</v>
+        <v>1840.967635557883</v>
       </c>
       <c r="BB5" t="n">
-        <v>-323406.7563488293</v>
+        <v>-323406.9503619066</v>
       </c>
       <c r="BC5" t="n">
-        <v>920.6998599856373</v>
+        <v>920.6993117505453</v>
       </c>
       <c r="BD5" t="n">
-        <v>1019.622469004632</v>
+        <v>1019.621179687479</v>
       </c>
       <c r="BE5" t="n">
-        <v>1.107442841384311</v>
+        <v>1.10744210044955</v>
       </c>
       <c r="BF5" t="n">
-        <v>0.936436544220814</v>
+        <v>0.9364378286384851</v>
       </c>
       <c r="BG5" t="n">
-        <v>170.9518397137049</v>
+        <v>170.9519690238077</v>
       </c>
       <c r="BH5" t="n">
-        <v>1685604.747945832</v>
+        <v>1685568.126431536</v>
       </c>
       <c r="BI5" t="n">
-        <v>5.932588889647192e-07</v>
+        <v>5.932717784104454e-07</v>
       </c>
       <c r="BJ5" t="n">
-        <v>1522069.297805758</v>
+        <v>1522037.247588207</v>
       </c>
       <c r="BK5" t="n">
-        <v>6.570003096715884e-07</v>
+        <v>6.570141444203037e-07</v>
       </c>
       <c r="BL5" t="n">
-        <v>0.002937490622591501</v>
+        <v>0.00293747721859136</v>
       </c>
       <c r="BM5" t="n">
-        <v>1.900275414738004e-05</v>
+        <v>1.900272557950027e-05</v>
       </c>
       <c r="BN5" t="n">
-        <v>0.0257827213382656</v>
+        <v>0.02578268017556692</v>
       </c>
       <c r="BO5" t="n">
-        <v>2.272758673576778</v>
+        <v>2.272747090294639</v>
       </c>
       <c r="BP5" t="inlineStr"/>
       <c r="BQ5" t="inlineStr"/>
       <c r="BR5" t="n">
-        <v>1625469.688857595</v>
+        <v>1625433.2547569</v>
       </c>
       <c r="BS5" t="n">
-        <v>57.67773378537485</v>
+        <v>57.67639342236885</v>
       </c>
       <c r="BT5" t="n">
-        <v>57.67773378537485</v>
+        <v>57.67639342236885</v>
       </c>
       <c r="BU5" t="n">
-        <v>448175.9483176969</v>
+        <v>448175.8571005159</v>
       </c>
       <c r="BV5" t="n">
-        <v>476357.8754181295</v>
+        <v>476357.8074324953</v>
       </c>
       <c r="BW5" t="n">
-        <v>1840.966337971765</v>
+        <v>1840.967635557883</v>
       </c>
       <c r="BX5" t="n">
-        <v>920.6998599856373</v>
+        <v>920.6993117505453</v>
       </c>
       <c r="BY5" t="n">
-        <v>1019.622469004632</v>
+        <v>1019.621179687479</v>
       </c>
       <c r="BZ5" t="n">
-        <v>170.9518397137049</v>
+        <v>170.9519690238077</v>
       </c>
       <c r="CA5" t="n">
-        <v>0.936436544220814</v>
+        <v>0.9364378286384851</v>
       </c>
       <c r="CB5" t="n">
-        <v>1.900275414738004e-05</v>
+        <v>1.900272557950027e-05</v>
       </c>
       <c r="CC5" t="n">
-        <v>0.0257827213382656</v>
+        <v>0.02578268017556692</v>
       </c>
       <c r="CD5" t="inlineStr">
         <is>
@@ -2822,102 +2822,102 @@
       </c>
       <c r="CF5" t="inlineStr"/>
       <c r="CG5" t="n">
-        <v>456.4266537273212</v>
+        <v>456.4396116623464</v>
       </c>
       <c r="CH5" t="n">
-        <v>2949167.256753977</v>
+        <v>2950110.344121861</v>
       </c>
       <c r="CI5" t="n">
-        <v>102.8207624481299</v>
+        <v>102.8526566547996</v>
       </c>
       <c r="CJ5" t="n">
-        <v>464622.2994906023</v>
+        <v>464631.7875374468</v>
       </c>
       <c r="CK5" t="n">
-        <v>493304.9039231629</v>
+        <v>493314.6669114157</v>
       </c>
       <c r="CL5" t="n">
-        <v>1840.966337971507</v>
+        <v>1840.967635557819</v>
       </c>
       <c r="CM5" t="n">
-        <v>-346961.2013418129</v>
+        <v>-346975.8857455432</v>
       </c>
       <c r="CN5" t="n">
-        <v>952.0767389408135</v>
+        <v>952.094891824714</v>
       </c>
       <c r="CO5" t="n">
-        <v>1072.434017646735</v>
+        <v>1072.46707680811</v>
       </c>
       <c r="CP5" t="n">
-        <v>1.126415522807352</v>
+        <v>1.126428768830698</v>
       </c>
       <c r="CQ5" t="n">
-        <v>0.9071343217814732</v>
+        <v>0.9071172642296209</v>
       </c>
       <c r="CR5" t="n">
-        <v>171.4722582670296</v>
+        <v>171.4727965688543</v>
       </c>
       <c r="CS5" t="n">
-        <v>3023211.667281724</v>
+        <v>3024168.431617772</v>
       </c>
       <c r="CT5" t="n">
-        <v>3.307740608513645e-07</v>
+        <v>3.306694129681965e-07</v>
       </c>
       <c r="CU5" t="n">
-        <v>2683922.234795744</v>
+        <v>2684740.052189045</v>
       </c>
       <c r="CV5" t="n">
-        <v>3.725890366850005e-07</v>
+        <v>3.724755397397354e-07</v>
       </c>
       <c r="CW5" t="n">
-        <v>0.003178382251129717</v>
+        <v>0.003178542658291291</v>
       </c>
       <c r="CX5" t="n">
-        <v>2.061277752750396e-05</v>
+        <v>2.061389068407235e-05</v>
       </c>
       <c r="CY5" t="n">
-        <v>0.02849554756121006</v>
+        <v>0.02849728148631422</v>
       </c>
       <c r="CZ5" t="n">
-        <v>3.41842974388428</v>
+        <v>3.42015938300639</v>
       </c>
       <c r="DA5" t="inlineStr"/>
       <c r="DB5" t="inlineStr"/>
       <c r="DC5" t="n">
-        <v>2949167.256753977</v>
+        <v>2950110.344121861</v>
       </c>
       <c r="DD5" t="n">
-        <v>102.8207624481299</v>
+        <v>102.8526566547996</v>
       </c>
       <c r="DE5" t="n">
-        <v>102.8207624481299</v>
+        <v>102.8526566547996</v>
       </c>
       <c r="DF5" t="n">
-        <v>464622.2994906023</v>
+        <v>464631.7875374468</v>
       </c>
       <c r="DG5" t="n">
-        <v>493304.9039231629</v>
+        <v>493314.6669114157</v>
       </c>
       <c r="DH5" t="n">
-        <v>1840.966337971507</v>
+        <v>1840.967635557819</v>
       </c>
       <c r="DI5" t="n">
-        <v>952.0767389408135</v>
+        <v>952.094891824714</v>
       </c>
       <c r="DJ5" t="n">
-        <v>1072.434017646735</v>
+        <v>1072.46707680811</v>
       </c>
       <c r="DK5" t="n">
-        <v>171.4722582670296</v>
+        <v>171.4727965688543</v>
       </c>
       <c r="DL5" t="n">
-        <v>0.9071343217814732</v>
+        <v>0.9071172642296209</v>
       </c>
       <c r="DM5" t="n">
-        <v>2.061277752750396e-05</v>
+        <v>2.061389068407235e-05</v>
       </c>
       <c r="DN5" t="n">
-        <v>0.02849554756121006</v>
+        <v>0.02849728148631422</v>
       </c>
       <c r="DO5" t="inlineStr">
         <is>
@@ -2929,40 +2929,40 @@
       </c>
       <c r="DQ5" t="inlineStr"/>
       <c r="DR5" t="n">
-        <v>0.2204992133873621</v>
+        <v>0.2204013680765203</v>
       </c>
       <c r="DS5" t="n">
-        <v>1.099445502658115</v>
+        <v>1.099730969920358</v>
       </c>
       <c r="DT5" t="n">
-        <v>4692637.410938793</v>
+        <v>4694648.738719262</v>
       </c>
       <c r="DU5" t="n">
-        <v>10.65999932430811</v>
+        <v>10.65999725096994</v>
       </c>
       <c r="DV5" t="n">
-        <v>476047.8480957093</v>
+        <v>476058.9030049462</v>
       </c>
       <c r="DW5" t="n">
-        <v>0.0328676992638086</v>
+        <v>0.03296213317790568</v>
       </c>
       <c r="DX5" t="n">
         <v>0</v>
       </c>
       <c r="DY5" t="n">
-        <v>0.01172474975661797</v>
+        <v>0.01172196731415109</v>
       </c>
       <c r="DZ5" t="n">
-        <v>0.009107777750327936</v>
+        <v>0.009089240236234926</v>
       </c>
       <c r="EA5" t="n">
-        <v>0.02609186551125709</v>
+        <v>0.02606520523674515</v>
       </c>
       <c r="EB5" t="n">
-        <v>0.0797920922820116</v>
+        <v>0.07983854596503685</v>
       </c>
       <c r="EC5" t="n">
-        <v>-4.619297839514314e-07</v>
+        <v>-4.965856748029296e-07</v>
       </c>
       <c r="ED5" t="n">
         <v>0</v>
@@ -3729,150 +3729,150 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.01980130068621652</v>
+        <v>0.01979882120425101</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0.01172129159082114</v>
+        <v>0.01172092194423158</v>
       </c>
       <c r="E2" t="n">
-        <v>0.04196859139198431</v>
+        <v>0.04197016482468759</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0.07349118366902196</v>
+        <v>0.07348990797317018</v>
       </c>
       <c r="H2" t="n">
-        <v>-3.889674760115813e-06</v>
+        <v>-4.204655697226389e-08</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>118.5642598745687</v>
+        <v>118.5081303288263</v>
       </c>
       <c r="K2" t="n">
-        <v>22.21672687818015</v>
+        <v>22.20620925011189</v>
       </c>
       <c r="L2" t="n">
-        <v>116.4641608668718</v>
+        <v>116.4090255296999</v>
       </c>
       <c r="M2" t="n">
-        <v>79.20000000000002</v>
+        <v>79.19999999999999</v>
       </c>
       <c r="N2" t="n">
-        <v>118.5642598745687</v>
+        <v>118.5081303288263</v>
       </c>
       <c r="O2" t="n">
-        <v>22.21672687818015</v>
+        <v>22.20620925011189</v>
       </c>
       <c r="P2" t="n">
-        <v>116.4641608668718</v>
+        <v>116.4090255296999</v>
       </c>
       <c r="Q2" t="n">
-        <v>79.20000000000002</v>
+        <v>79.19999999999999</v>
       </c>
       <c r="R2" t="n">
-        <v>453.4667728538431</v>
+        <v>453.4757591537251</v>
       </c>
       <c r="S2" t="n">
-        <v>2831494.656334256</v>
+        <v>2832155.096285358</v>
       </c>
       <c r="T2" t="n">
-        <v>99.25248892326084</v>
+        <v>99.27507677616963</v>
       </c>
       <c r="U2" t="n">
-        <v>462129.3707899103</v>
+        <v>462135.8625086189</v>
       </c>
       <c r="V2" t="n">
-        <v>490657.5687933224</v>
+        <v>490664.2221760797</v>
       </c>
       <c r="W2" t="n">
-        <v>1837.707528152913</v>
+        <v>1837.707528152632</v>
       </c>
       <c r="X2" t="n">
-        <v>-342681.7334473921</v>
+        <v>-342691.5942554506</v>
       </c>
       <c r="Y2" t="n">
-        <v>948.5487152197353</v>
+        <v>948.5615812174253</v>
       </c>
       <c r="Z2" t="n">
-        <v>1067.664068553346</v>
+        <v>1067.687735251104</v>
       </c>
       <c r="AA2" t="n">
-        <v>1.125576421561034</v>
+        <v>1.125586104679452</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.908140163160186</v>
+        <v>0.908127313166868</v>
       </c>
       <c r="AC2" t="n">
-        <v>170.9932318403062</v>
+        <v>170.9934463893318</v>
       </c>
       <c r="AD2" t="n">
-        <v>2902012.292361923</v>
+        <v>2902680.015586653</v>
       </c>
       <c r="AE2" t="n">
-        <v>3.445884783575842e-07</v>
+        <v>3.445092103264068e-07</v>
       </c>
       <c r="AF2" t="n">
-        <v>2578245.454304378</v>
+        <v>2578816.497040257</v>
       </c>
       <c r="AG2" t="n">
-        <v>3.878606663808914e-07</v>
+        <v>3.877747800774943e-07</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.003179945737839582</v>
+        <v>0.003180068083544039</v>
       </c>
       <c r="AI2" t="n">
-        <v>2.043089802930722e-05</v>
+        <v>2.043167092226909e-05</v>
       </c>
       <c r="AJ2" t="n">
-        <v>0.02816502258580502</v>
+        <v>0.02816622765939236</v>
       </c>
       <c r="AK2" t="n">
-        <v>3.203267779017572</v>
+        <v>3.204233747545305</v>
       </c>
       <c r="AL2" t="inlineStr"/>
       <c r="AM2" t="inlineStr"/>
       <c r="AN2" t="n">
-        <v>2831494.656334256</v>
+        <v>2832155.096285358</v>
       </c>
       <c r="AO2" t="n">
-        <v>99.25248892326084</v>
+        <v>99.27507677616963</v>
       </c>
       <c r="AP2" t="n">
-        <v>99.25248892326084</v>
+        <v>99.27507677616963</v>
       </c>
       <c r="AQ2" t="n">
-        <v>462129.3707899103</v>
+        <v>462135.8625086189</v>
       </c>
       <c r="AR2" t="n">
-        <v>490657.5687933224</v>
+        <v>490664.2221760797</v>
       </c>
       <c r="AS2" t="n">
-        <v>1837.707528152913</v>
+        <v>1837.707528152632</v>
       </c>
       <c r="AT2" t="n">
-        <v>948.5487152197353</v>
+        <v>948.5615812174253</v>
       </c>
       <c r="AU2" t="n">
-        <v>1067.664068553346</v>
+        <v>1067.687735251104</v>
       </c>
       <c r="AV2" t="n">
-        <v>170.9932318403062</v>
+        <v>170.9934463893318</v>
       </c>
       <c r="AW2" t="n">
-        <v>0.908140163160186</v>
+        <v>0.908127313166868</v>
       </c>
       <c r="AX2" t="n">
-        <v>2.043089802930722e-05</v>
+        <v>2.043167092226909e-05</v>
       </c>
       <c r="AY2" t="n">
-        <v>0.02816502258580502</v>
+        <v>0.02816622765939236</v>
       </c>
       <c r="AZ2" t="inlineStr">
         <is>
@@ -3884,102 +3884,102 @@
       </c>
       <c r="BB2" t="inlineStr"/>
       <c r="BC2" t="n">
-        <v>463.1499999986578</v>
+        <v>463.1499999987764</v>
       </c>
       <c r="BD2" t="n">
-        <v>3619999.999950372</v>
+        <v>3619999.999964131</v>
       </c>
       <c r="BE2" t="n">
-        <v>126.17109542408</v>
+        <v>126.1710954245631</v>
       </c>
       <c r="BF2" t="n">
-        <v>468995.1117077454</v>
+        <v>468995.1117078174</v>
       </c>
       <c r="BG2" t="n">
-        <v>497686.3106529794</v>
+        <v>497686.3106530505</v>
       </c>
       <c r="BH2" t="n">
-        <v>1837.707528152808</v>
+        <v>1837.707528152727</v>
       </c>
       <c r="BI2" t="n">
-        <v>-353447.9310085271</v>
+        <v>-353447.9310086363</v>
       </c>
       <c r="BJ2" t="n">
-        <v>962.3636476150148</v>
+        <v>962.3636476152021</v>
       </c>
       <c r="BK2" t="n">
-        <v>1094.306525493691</v>
+        <v>1094.306525494122</v>
       </c>
       <c r="BL2" t="n">
-        <v>1.137102932145935</v>
+        <v>1.137102932146161</v>
       </c>
       <c r="BM2" t="n">
-        <v>0.8942337187250198</v>
+        <v>0.8942337187247649</v>
       </c>
       <c r="BN2" t="n">
-        <v>171.3408636171301</v>
+        <v>171.3408636171266</v>
       </c>
       <c r="BO2" t="n">
-        <v>3704092.101362972</v>
+        <v>3704092.101377005</v>
       </c>
       <c r="BP2" t="n">
-        <v>2.699716887795625e-07</v>
+        <v>2.699716887785398e-07</v>
       </c>
       <c r="BQ2" t="n">
-        <v>3257481.795753201</v>
+        <v>3257481.795764893</v>
       </c>
       <c r="BR2" t="n">
-        <v>3.069855989076304e-07</v>
+        <v>3.069855989065286e-07</v>
       </c>
       <c r="BS2" t="n">
-        <v>0.00332178163873304</v>
+        <v>0.003321781638736081</v>
       </c>
       <c r="BT2" t="n">
-        <v>2.134925593332515e-05</v>
+        <v>2.134925593334009e-05</v>
       </c>
       <c r="BU2" t="n">
-        <v>0.0295272176624014</v>
+        <v>0.02952721766242114</v>
       </c>
       <c r="BV2" t="n">
-        <v>6.146178711981554</v>
+        <v>6.146178711973488</v>
       </c>
       <c r="BW2" t="inlineStr"/>
       <c r="BX2" t="inlineStr"/>
       <c r="BY2" t="n">
-        <v>3619999.999950372</v>
+        <v>3619999.999964131</v>
       </c>
       <c r="BZ2" t="n">
-        <v>126.17109542408</v>
+        <v>126.1710954245631</v>
       </c>
       <c r="CA2" t="n">
-        <v>126.17109542408</v>
+        <v>126.1710954245631</v>
       </c>
       <c r="CB2" t="n">
-        <v>468995.1117077454</v>
+        <v>468995.1117078174</v>
       </c>
       <c r="CC2" t="n">
-        <v>497686.3106529794</v>
+        <v>497686.3106530505</v>
       </c>
       <c r="CD2" t="n">
-        <v>1837.707528152808</v>
+        <v>1837.707528152727</v>
       </c>
       <c r="CE2" t="n">
-        <v>962.3636476150148</v>
+        <v>962.3636476152021</v>
       </c>
       <c r="CF2" t="n">
-        <v>1094.306525493691</v>
+        <v>1094.306525494122</v>
       </c>
       <c r="CG2" t="n">
-        <v>171.3408636171301</v>
+        <v>171.3408636171266</v>
       </c>
       <c r="CH2" t="n">
-        <v>0.8942337187250198</v>
+        <v>0.8942337187247649</v>
       </c>
       <c r="CI2" t="n">
-        <v>2.134925593332515e-05</v>
+        <v>2.134925593334009e-05</v>
       </c>
       <c r="CJ2" t="n">
-        <v>0.0295272176624014</v>
+        <v>0.02952721766242114</v>
       </c>
       <c r="CK2" t="inlineStr">
         <is>
@@ -3991,102 +3991,102 @@
       </c>
       <c r="CM2" t="inlineStr"/>
       <c r="CN2" t="n">
-        <v>463.1499999986578</v>
+        <v>463.1499999987764</v>
       </c>
       <c r="CO2" t="n">
-        <v>3619999.999950372</v>
+        <v>3619999.999964131</v>
       </c>
       <c r="CP2" t="n">
-        <v>126.17109542408</v>
+        <v>126.1710954245631</v>
       </c>
       <c r="CQ2" t="n">
-        <v>468995.1117077454</v>
+        <v>468995.1117078174</v>
       </c>
       <c r="CR2" t="n">
-        <v>497686.3106529794</v>
+        <v>497686.3106530505</v>
       </c>
       <c r="CS2" t="n">
-        <v>1837.707528152808</v>
+        <v>1837.707528152727</v>
       </c>
       <c r="CT2" t="n">
-        <v>-353447.9310085271</v>
+        <v>-353447.9310086363</v>
       </c>
       <c r="CU2" t="n">
-        <v>962.3636476150148</v>
+        <v>962.3636476152021</v>
       </c>
       <c r="CV2" t="n">
-        <v>1094.306525493691</v>
+        <v>1094.306525494122</v>
       </c>
       <c r="CW2" t="n">
-        <v>1.137102932145935</v>
+        <v>1.137102932146161</v>
       </c>
       <c r="CX2" t="n">
-        <v>0.8942337187250198</v>
+        <v>0.8942337187247649</v>
       </c>
       <c r="CY2" t="n">
-        <v>171.3408636171301</v>
+        <v>171.3408636171266</v>
       </c>
       <c r="CZ2" t="n">
-        <v>3704092.101362972</v>
+        <v>3704092.101377005</v>
       </c>
       <c r="DA2" t="n">
-        <v>2.699716887795625e-07</v>
+        <v>2.699716887785398e-07</v>
       </c>
       <c r="DB2" t="n">
-        <v>3257481.795753201</v>
+        <v>3257481.795764893</v>
       </c>
       <c r="DC2" t="n">
-        <v>3.069855989076304e-07</v>
+        <v>3.069855989065286e-07</v>
       </c>
       <c r="DD2" t="n">
-        <v>0.00332178163873304</v>
+        <v>0.003321781638736081</v>
       </c>
       <c r="DE2" t="n">
-        <v>2.134925593332515e-05</v>
+        <v>2.134925593334009e-05</v>
       </c>
       <c r="DF2" t="n">
-        <v>0.0295272176624014</v>
+        <v>0.02952721766242114</v>
       </c>
       <c r="DG2" t="n">
-        <v>6.146178711981554</v>
+        <v>6.146178711973488</v>
       </c>
       <c r="DH2" t="inlineStr"/>
       <c r="DI2" t="inlineStr"/>
       <c r="DJ2" t="n">
-        <v>3619999.999950372</v>
+        <v>3619999.999964131</v>
       </c>
       <c r="DK2" t="n">
-        <v>126.17109542408</v>
+        <v>126.1710954245631</v>
       </c>
       <c r="DL2" t="n">
-        <v>126.17109542408</v>
+        <v>126.1710954245631</v>
       </c>
       <c r="DM2" t="n">
-        <v>468995.1117077454</v>
+        <v>468995.1117078174</v>
       </c>
       <c r="DN2" t="n">
-        <v>497686.3106529794</v>
+        <v>497686.3106530505</v>
       </c>
       <c r="DO2" t="n">
-        <v>1837.707528152808</v>
+        <v>1837.707528152727</v>
       </c>
       <c r="DP2" t="n">
-        <v>962.3636476150148</v>
+        <v>962.3636476152021</v>
       </c>
       <c r="DQ2" t="n">
-        <v>1094.306525493691</v>
+        <v>1094.306525494122</v>
       </c>
       <c r="DR2" t="n">
-        <v>171.3408636171301</v>
+        <v>171.3408636171266</v>
       </c>
       <c r="DS2" t="n">
-        <v>0.8942337187250198</v>
+        <v>0.8942337187247649</v>
       </c>
       <c r="DT2" t="n">
-        <v>2.134925593332515e-05</v>
+        <v>2.134925593334009e-05</v>
       </c>
       <c r="DU2" t="n">
-        <v>0.0295272176624014</v>
+        <v>0.02952721766242114</v>
       </c>
       <c r="DV2" t="inlineStr">
         <is>
@@ -4098,37 +4098,37 @@
       </c>
       <c r="DX2" t="inlineStr"/>
       <c r="DY2" t="n">
-        <v>0.01990571253603948</v>
+        <v>0.01990701045110415</v>
       </c>
       <c r="DZ2" t="n">
         <v>0</v>
       </c>
       <c r="EA2" t="n">
-        <v>0.01171974176750878</v>
+        <v>0.01171937504463072</v>
       </c>
       <c r="EB2" t="n">
-        <v>0.04195313545620567</v>
+        <v>0.04195472083317529</v>
       </c>
       <c r="EC2" t="n">
         <v>0</v>
       </c>
       <c r="ED2" t="n">
-        <v>0.07357858975975393</v>
+        <v>0.07358110632891016</v>
       </c>
       <c r="EE2" t="n">
-        <v>-0.07357858975975393</v>
+        <v>-0.07358110632891016</v>
       </c>
       <c r="EF2" t="n">
-        <v>0.6933856890037499</v>
+        <v>0.6930565634603174</v>
       </c>
       <c r="EG2" t="n">
-        <v>0.6933856890037499</v>
+        <v>0.6930565634603174</v>
       </c>
       <c r="EH2" t="n">
-        <v>5974463.818364521</v>
+        <v>5980558.104971689</v>
       </c>
       <c r="EI2" t="n">
-        <v>10.65999985532357</v>
+        <v>10.6600008655268</v>
       </c>
       <c r="EJ2" t="n">
         <v>497686.3106530505</v>
@@ -4137,25 +4137,25 @@
         <v>0</v>
       </c>
       <c r="EL2" t="n">
-        <v>446.1816088011838</v>
+        <v>445.8350650867214</v>
       </c>
       <c r="EM2" t="n">
-        <v>-20.46919387496283</v>
+        <v>-20.45821181387751</v>
       </c>
       <c r="EN2" t="n">
-        <v>0.005053706115159042</v>
+        <v>0.005049283615127915</v>
       </c>
       <c r="EO2" t="n">
         <v>0</v>
       </c>
       <c r="EP2" t="n">
-        <v>0.01071126237227035</v>
+        <v>0.01070363045290857</v>
       </c>
       <c r="EQ2" t="n">
         <v>0</v>
       </c>
       <c r="ER2" t="n">
-        <v>0.002991518786002202</v>
+        <v>0.002989180947525031</v>
       </c>
     </row>
     <row r="3">
@@ -4163,150 +4163,150 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0328676992638086</v>
+        <v>0.03296213317790568</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.01172474975661797</v>
+        <v>0.01172196731415109</v>
       </c>
       <c r="E3" t="n">
-        <v>0.009107777750327936</v>
+        <v>0.009089240236234926</v>
       </c>
       <c r="F3" t="n">
-        <v>0.02609186551125709</v>
+        <v>0.02606520523674515</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0797920922820116</v>
+        <v>0.07983854596503685</v>
       </c>
       <c r="H3" t="n">
-        <v>-4.619297839514314e-07</v>
+        <v>-4.965856748029296e-07</v>
       </c>
       <c r="I3" t="n">
-        <v>185.7797396241413</v>
+        <v>185.7727854477948</v>
       </c>
       <c r="J3" t="n">
-        <v>37.36492816017142</v>
+        <v>37.33859131266407</v>
       </c>
       <c r="K3" t="n">
-        <v>32.66665150429738</v>
+        <v>32.64305732274362</v>
       </c>
       <c r="L3" t="n">
-        <v>18.13912169625522</v>
+        <v>18.12736080730525</v>
       </c>
       <c r="M3" t="n">
-        <v>29.04251595417455</v>
+        <v>29.04431426305131</v>
       </c>
       <c r="N3" t="n">
-        <v>170.793696897007</v>
+        <v>170.7939038556879</v>
       </c>
       <c r="O3" t="n">
-        <v>32.66665150429738</v>
+        <v>32.64305732274362</v>
       </c>
       <c r="P3" t="n">
-        <v>-167.6406179278861</v>
+        <v>-167.6454246404895</v>
       </c>
       <c r="Q3" t="n">
-        <v>-78.97345268455423</v>
+        <v>-78.98153005139142</v>
       </c>
       <c r="R3" t="n">
-        <v>437.6877106818002</v>
+        <v>437.7001814968526</v>
       </c>
       <c r="S3" t="n">
-        <v>1830723.762626376</v>
+        <v>1831377.329812168</v>
       </c>
       <c r="T3" t="n">
-        <v>64.88305381696689</v>
+        <v>64.90552364786778</v>
       </c>
       <c r="U3" t="n">
-        <v>450503.914528459</v>
+        <v>450513.340744416</v>
       </c>
       <c r="V3" t="n">
-        <v>478719.6604733214</v>
+        <v>478729.3881142507</v>
       </c>
       <c r="W3" t="n">
-        <v>1838.692343556447</v>
+        <v>1838.691558491637</v>
       </c>
       <c r="X3" t="n">
-        <v>-326053.3820260535</v>
+        <v>-326066.2407542696</v>
       </c>
       <c r="Y3" t="n">
-        <v>925.7421860914026</v>
+        <v>925.7601880301049</v>
       </c>
       <c r="Z3" t="n">
-        <v>1028.297886474233</v>
+        <v>1028.326719178194</v>
       </c>
       <c r="AA3" t="n">
-        <v>1.110782139912877</v>
+        <v>1.110791685011144</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.930574605244775</v>
+        <v>0.9305580325261882</v>
       </c>
       <c r="AC3" t="n">
-        <v>170.7936969788664</v>
+        <v>170.7939041916059</v>
       </c>
       <c r="AD3" t="n">
-        <v>1892670.273197662</v>
+        <v>1893330.323203734</v>
       </c>
       <c r="AE3" t="n">
-        <v>5.283540478027916e-07</v>
+        <v>5.281698537991429e-07</v>
       </c>
       <c r="AF3" t="n">
-        <v>1703907.728788394</v>
+        <v>1704487.302841792</v>
       </c>
       <c r="AG3" t="n">
-        <v>5.868862398500152e-07</v>
+        <v>5.866866818736392e-07</v>
       </c>
       <c r="AH3" t="n">
-        <v>0.002987035133807928</v>
+        <v>0.002987159512920402</v>
       </c>
       <c r="AI3" t="n">
-        <v>1.923550349238876e-05</v>
+        <v>1.923632683649776e-05</v>
       </c>
       <c r="AJ3" t="n">
-        <v>0.02618226629480995</v>
+        <v>0.0261837244080992</v>
       </c>
       <c r="AK3" t="n">
-        <v>2.364312578902904</v>
+        <v>2.364651311555132</v>
       </c>
       <c r="AL3" t="inlineStr"/>
       <c r="AM3" t="inlineStr"/>
       <c r="AN3" t="n">
-        <v>1830723.762626376</v>
+        <v>1831377.329812168</v>
       </c>
       <c r="AO3" t="n">
-        <v>64.88305381696689</v>
+        <v>64.90552364786778</v>
       </c>
       <c r="AP3" t="n">
-        <v>64.88305381696689</v>
+        <v>64.90552364786778</v>
       </c>
       <c r="AQ3" t="n">
-        <v>450503.914528459</v>
+        <v>450513.340744416</v>
       </c>
       <c r="AR3" t="n">
-        <v>478719.6604733214</v>
+        <v>478729.3881142507</v>
       </c>
       <c r="AS3" t="n">
-        <v>1838.692343556447</v>
+        <v>1838.691558491637</v>
       </c>
       <c r="AT3" t="n">
-        <v>925.7421860914026</v>
+        <v>925.7601880301049</v>
       </c>
       <c r="AU3" t="n">
-        <v>1028.297886474233</v>
+        <v>1028.326719178194</v>
       </c>
       <c r="AV3" t="n">
-        <v>170.7936969788664</v>
+        <v>170.7939041916059</v>
       </c>
       <c r="AW3" t="n">
-        <v>0.930574605244775</v>
+        <v>0.9305580325261882</v>
       </c>
       <c r="AX3" t="n">
-        <v>1.923550349238876e-05</v>
+        <v>1.923632683649776e-05</v>
       </c>
       <c r="AY3" t="n">
-        <v>0.02618226629480995</v>
+        <v>0.0261837244080992</v>
       </c>
       <c r="AZ3" t="inlineStr">
         <is>
@@ -4318,102 +4318,102 @@
       </c>
       <c r="BB3" t="inlineStr"/>
       <c r="BC3" t="n">
-        <v>438.5765166977315</v>
+        <v>438.5877709070865</v>
       </c>
       <c r="BD3" t="n">
-        <v>1876562.854480083</v>
+        <v>1877166.90059507</v>
       </c>
       <c r="BE3" t="n">
-        <v>66.45428273595266</v>
+        <v>66.47505170119113</v>
       </c>
       <c r="BF3" t="n">
-        <v>451179.325836979</v>
+        <v>451187.8055358151</v>
       </c>
       <c r="BG3" t="n">
-        <v>479417.7294013716</v>
+        <v>479426.4733150149</v>
       </c>
       <c r="BH3" t="n">
-        <v>1838.6923435567</v>
+        <v>1838.691558491874</v>
       </c>
       <c r="BI3" t="n">
-        <v>-326989.5539145143</v>
+        <v>-327001.158709613</v>
       </c>
       <c r="BJ3" t="n">
-        <v>927.0155415352973</v>
+        <v>927.0318033444798</v>
       </c>
       <c r="BK3" t="n">
-        <v>1030.32359798759</v>
+        <v>1030.349875315029</v>
       </c>
       <c r="BL3" t="n">
-        <v>1.111441558230186</v>
+        <v>1.111450407200492</v>
       </c>
       <c r="BM3" t="n">
-        <v>0.9294344800685711</v>
+        <v>0.929419326782343</v>
       </c>
       <c r="BN3" t="n">
-        <v>170.8142720513213</v>
+        <v>170.8144388521347</v>
       </c>
       <c r="BO3" t="n">
-        <v>1938970.866990092</v>
+        <v>1939580.641806826</v>
       </c>
       <c r="BP3" t="n">
-        <v>5.157375064393423e-07</v>
+        <v>5.15575366368085e-07</v>
       </c>
       <c r="BQ3" t="n">
-        <v>1744554.945450871</v>
+        <v>1745089.685730755</v>
       </c>
       <c r="BR3" t="n">
-        <v>5.732120977946929e-07</v>
+        <v>5.730364508923509e-07</v>
       </c>
       <c r="BS3" t="n">
-        <v>0.002995460312621164</v>
+        <v>0.002995576076842247</v>
       </c>
       <c r="BT3" t="n">
-        <v>1.929385513503042e-05</v>
+        <v>1.92946092129158e-05</v>
       </c>
       <c r="BU3" t="n">
-        <v>0.02628584021082899</v>
+        <v>0.0262871667964243</v>
       </c>
       <c r="BV3" t="n">
-        <v>2.388671323315003</v>
+        <v>2.388993614071786</v>
       </c>
       <c r="BW3" t="inlineStr"/>
       <c r="BX3" t="inlineStr"/>
       <c r="BY3" t="n">
-        <v>1876562.854480083</v>
+        <v>1877166.90059507</v>
       </c>
       <c r="BZ3" t="n">
-        <v>66.45428273595266</v>
+        <v>66.47505170119113</v>
       </c>
       <c r="CA3" t="n">
-        <v>66.45428273595266</v>
+        <v>66.47505170119113</v>
       </c>
       <c r="CB3" t="n">
-        <v>451179.325836979</v>
+        <v>451187.8055358151</v>
       </c>
       <c r="CC3" t="n">
-        <v>479417.7294013716</v>
+        <v>479426.4733150149</v>
       </c>
       <c r="CD3" t="n">
-        <v>1838.6923435567</v>
+        <v>1838.691558491874</v>
       </c>
       <c r="CE3" t="n">
-        <v>927.0155415352973</v>
+        <v>927.0318033444798</v>
       </c>
       <c r="CF3" t="n">
-        <v>1030.32359798759</v>
+        <v>1030.349875315029</v>
       </c>
       <c r="CG3" t="n">
-        <v>170.8142720513213</v>
+        <v>170.8144388521347</v>
       </c>
       <c r="CH3" t="n">
-        <v>0.9294344800685711</v>
+        <v>0.929419326782343</v>
       </c>
       <c r="CI3" t="n">
-        <v>1.929385513503042e-05</v>
+        <v>1.92946092129158e-05</v>
       </c>
       <c r="CJ3" t="n">
-        <v>0.02628584021082899</v>
+        <v>0.0262871667964243</v>
       </c>
       <c r="CK3" t="inlineStr">
         <is>
@@ -4425,102 +4425,102 @@
       </c>
       <c r="CM3" t="inlineStr"/>
       <c r="CN3" t="n">
-        <v>456.870952130001</v>
+        <v>456.8844361503328</v>
       </c>
       <c r="CO3" t="n">
-        <v>3058016.392935408</v>
+        <v>3059098.10526875</v>
       </c>
       <c r="CP3" t="n">
-        <v>106.8524588375607</v>
+        <v>106.8894769712763</v>
       </c>
       <c r="CQ3" t="n">
-        <v>464685.8489550681</v>
+        <v>464695.4034258843</v>
       </c>
       <c r="CR3" t="n">
-        <v>493304.9039230428</v>
+        <v>493314.666911389</v>
       </c>
       <c r="CS3" t="n">
-        <v>1838.692343556472</v>
+        <v>1838.691558491648</v>
       </c>
       <c r="CT3" t="n">
-        <v>-346740.2177517454</v>
+        <v>-346754.8890444443</v>
       </c>
       <c r="CU3" t="n">
-        <v>953.201531836291</v>
+        <v>953.2209413459876</v>
       </c>
       <c r="CV3" t="n">
-        <v>1075.801501575035</v>
+        <v>1075.83864706782</v>
       </c>
       <c r="CW3" t="n">
-        <v>1.128619148882988</v>
+        <v>1.128635136308159</v>
       </c>
       <c r="CX3" t="n">
-        <v>0.9042442494176749</v>
+        <v>0.9042241505775809</v>
       </c>
       <c r="CY3" t="n">
-        <v>171.2068484868442</v>
+        <v>171.207164847422</v>
       </c>
       <c r="CZ3" t="n">
-        <v>3132036.296833836</v>
+        <v>3133132.943350279</v>
       </c>
       <c r="DA3" t="n">
-        <v>3.192811018859828e-07</v>
+        <v>3.191693484064846e-07</v>
       </c>
       <c r="DB3" t="n">
-        <v>2775104.693140872</v>
+        <v>2776037.040277665</v>
       </c>
       <c r="DC3" t="n">
-        <v>3.603467654649803e-07</v>
+        <v>3.60225741044139e-07</v>
       </c>
       <c r="DD3" t="n">
-        <v>0.003214407868481313</v>
+        <v>0.003214609757835316</v>
       </c>
       <c r="DE3" t="n">
-        <v>2.070850682738067e-05</v>
+        <v>2.070975438011819e-05</v>
       </c>
       <c r="DF3" t="n">
-        <v>0.02860670421699672</v>
+        <v>0.02860858259688217</v>
       </c>
       <c r="DG3" t="n">
-        <v>3.622711643980225</v>
+        <v>3.625180120699643</v>
       </c>
       <c r="DH3" t="inlineStr"/>
       <c r="DI3" t="inlineStr"/>
       <c r="DJ3" t="n">
-        <v>3058016.392935408</v>
+        <v>3059098.10526875</v>
       </c>
       <c r="DK3" t="n">
-        <v>106.8524588375607</v>
+        <v>106.8894769712763</v>
       </c>
       <c r="DL3" t="n">
-        <v>106.8524588375607</v>
+        <v>106.8894769712763</v>
       </c>
       <c r="DM3" t="n">
-        <v>464685.8489550681</v>
+        <v>464695.4034258843</v>
       </c>
       <c r="DN3" t="n">
-        <v>493304.9039230428</v>
+        <v>493314.666911389</v>
       </c>
       <c r="DO3" t="n">
-        <v>1838.692343556472</v>
+        <v>1838.691558491648</v>
       </c>
       <c r="DP3" t="n">
-        <v>953.201531836291</v>
+        <v>953.2209413459876</v>
       </c>
       <c r="DQ3" t="n">
-        <v>1075.801501575035</v>
+        <v>1075.83864706782</v>
       </c>
       <c r="DR3" t="n">
-        <v>171.2068484868442</v>
+        <v>171.207164847422</v>
       </c>
       <c r="DS3" t="n">
-        <v>0.9042442494176749</v>
+        <v>0.9042241505775809</v>
       </c>
       <c r="DT3" t="n">
-        <v>2.070850682738067e-05</v>
+        <v>2.070975438011819e-05</v>
       </c>
       <c r="DU3" t="n">
-        <v>0.02860670421699672</v>
+        <v>0.02860858259688217</v>
       </c>
       <c r="DV3" t="inlineStr">
         <is>
@@ -4532,64 +4532,64 @@
       </c>
       <c r="DX3" t="inlineStr"/>
       <c r="DY3" t="n">
-        <v>0.0206162575201694</v>
+        <v>0.02066543271955217</v>
       </c>
       <c r="DZ3" t="n">
         <v>0</v>
       </c>
       <c r="EA3" t="n">
-        <v>0.01172009780977423</v>
+        <v>0.01171734765875199</v>
       </c>
       <c r="EB3" t="n">
-        <v>0.01039353312191402</v>
+        <v>0.01037671626204016</v>
       </c>
       <c r="EC3" t="n">
-        <v>0.03138370899855804</v>
+        <v>0.03136807044420025</v>
       </c>
       <c r="ED3" t="n">
-        <v>0.07411359745041569</v>
+        <v>0.07412756708454457</v>
       </c>
       <c r="EE3" t="n">
-        <v>-0.07411359744106182</v>
+        <v>-0.07412756708454457</v>
       </c>
       <c r="EF3" t="n">
-        <v>0.2187722897338235</v>
+        <v>0.2186178218092352</v>
       </c>
       <c r="EG3" t="n">
-        <v>0.9999999995207119</v>
+        <v>0.9999999980331973</v>
       </c>
       <c r="EH3" t="n">
-        <v>4842457.108973747</v>
+        <v>4844759.759628373</v>
       </c>
       <c r="EI3" t="n">
-        <v>10.65999984770521</v>
+        <v>10.65999792170842</v>
       </c>
       <c r="EJ3" t="n">
-        <v>476047.8480957093</v>
+        <v>476058.9030049462</v>
       </c>
       <c r="EK3" t="n">
         <v>0</v>
       </c>
       <c r="EL3" t="n">
-        <v>984.7639288936625</v>
+        <v>985.6660745106637</v>
       </c>
       <c r="EM3" t="n">
-        <v>-51.52128025557745</v>
+        <v>-51.62137603518779</v>
       </c>
       <c r="EN3" t="n">
-        <v>0.01705223956615012</v>
+        <v>0.01710710071037147</v>
       </c>
       <c r="EO3" t="n">
         <v>0</v>
       </c>
       <c r="EP3" t="n">
-        <v>0.004725247327696499</v>
+        <v>0.004717247735843015</v>
       </c>
       <c r="EQ3" t="n">
-        <v>0.01353683864071505</v>
+        <v>0.01352764666700593</v>
       </c>
       <c r="ER3" t="n">
-        <v>0.006082970398940005</v>
+        <v>0.006083613408287504</v>
       </c>
     </row>
   </sheetData>
@@ -4623,7 +4623,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.6830064125517721</v>
+        <v>0.6833006886473332</v>
       </c>
     </row>
   </sheetData>
@@ -4882,28 +4882,28 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.03501859258296947</v>
+        <v>0.03502355267595494</v>
       </c>
       <c r="C2" t="n">
-        <v>0.05836432097161578</v>
+        <v>0.05837258779325816</v>
       </c>
       <c r="D2" t="n">
-        <v>0.03845219259313437</v>
+        <v>0.03845794556513049</v>
       </c>
       <c r="E2" t="n">
-        <v>0.05493072096145088</v>
+        <v>0.0549381949040826</v>
       </c>
       <c r="F2" t="n">
-        <v>0.007779513775317581</v>
+        <v>0.00778965968595588</v>
       </c>
       <c r="G2" t="n">
-        <v>0.01037268503375677</v>
+        <v>0.01038621291460784</v>
       </c>
       <c r="H2" t="n">
-        <v>0.001457735518056761</v>
+        <v>0.001459636672129838</v>
       </c>
       <c r="I2" t="n">
-        <v>0.002329564947917464</v>
+        <v>0.002332460549695806</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -4911,13 +4911,13 @@
         </is>
       </c>
       <c r="K2" t="n">
-        <v>20.46919387496283</v>
+        <v>20.45821181387751</v>
       </c>
       <c r="L2" t="n">
-        <v>79.20000000000002</v>
+        <v>79.19999999999999</v>
       </c>
       <c r="M2" t="n">
-        <v>-29.36540306251859</v>
+        <v>-29.37089409306124</v>
       </c>
       <c r="N2" t="n">
         <v>0.01200896</v>
@@ -4926,7 +4926,7 @@
         <v>45</v>
       </c>
       <c r="P2" t="n">
-        <v>7.288677590283858e-05</v>
+        <v>7.298183360649198e-05</v>
       </c>
       <c r="Q2" t="n">
         <v>0</v>
@@ -4941,85 +4941,85 @@
         <v>2</v>
       </c>
       <c r="U2" t="n">
-        <v>0.009039899510884249</v>
+        <v>0.009051201042235821</v>
       </c>
       <c r="V2" t="n">
-        <v>0.04669145677729263</v>
+        <v>0.04669807023460655</v>
       </c>
       <c r="W2" t="n">
-        <v>0.04669145677729263</v>
+        <v>0.04669807023460655</v>
       </c>
       <c r="X2" t="n">
-        <v>0.04669145677729263</v>
+        <v>0.04669807023460655</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.03845219259313437</v>
+        <v>0.03845794556513049</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.05493072096145088</v>
+        <v>0.0549381949040826</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.05836432097161578</v>
+        <v>0.05837258779325816</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.05493072096145088</v>
+        <v>0.0549381949040826</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.05493072096145088</v>
+        <v>0.0549381949040826</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.6000000000000001</v>
+        <v>0.6000000000000008</v>
       </c>
       <c r="AE2" t="n">
-        <v>0.7000125234132506</v>
+        <v>0.700022008955241</v>
       </c>
       <c r="AF2" t="n">
-        <v>0.7000125234132506</v>
+        <v>0.700022008955241</v>
       </c>
       <c r="AG2" t="n">
-        <v>0.006848961438561822</v>
+        <v>0.00685090177305115</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.004834323585026126</v>
+        <v>0.004835513281355344</v>
       </c>
       <c r="AI2" t="n">
-        <v>0.0009058619084949682</v>
+        <v>0.0009060848353570968</v>
       </c>
       <c r="AJ2" t="n">
-        <v>0.01991212837848141</v>
+        <v>0.01991464222812767</v>
       </c>
       <c r="AK2" t="n">
-        <v>0.02334572838864631</v>
+        <v>0.02334903511730322</v>
       </c>
       <c r="AL2" t="n">
-        <v>0.01647852836831651</v>
+        <v>0.01648024933895211</v>
       </c>
       <c r="AM2" t="n">
-        <v>0.01647852836831651</v>
+        <v>0.01648024933895211</v>
       </c>
       <c r="AN2" t="n">
-        <v>-0.3629960332272993</v>
+        <v>-20.77877730306741</v>
       </c>
       <c r="AO2" t="n">
-        <v>1.919669623986417</v>
+        <v>1.917411321321791</v>
       </c>
       <c r="AP2" t="n">
-        <v>0.75</v>
+        <v>0.7500000000000001</v>
       </c>
       <c r="AQ2" t="n">
         <v>1.333333333333333</v>
       </c>
       <c r="AR2" t="n">
-        <v>0.2245864923437035</v>
+        <v>0.2245727647673469</v>
       </c>
       <c r="AS2" t="n">
-        <v>0.05000000000000036</v>
+        <v>0.05000000000000006</v>
       </c>
       <c r="AT2" t="n">
         <v>0</v>
       </c>
       <c r="AU2" t="n">
-        <v>1.15774844805546</v>
+        <v>1.15624049870091</v>
       </c>
     </row>
     <row r="3">
@@ -5027,28 +5027,28 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.03845219259316247</v>
+        <v>0.03845794556509228</v>
       </c>
       <c r="C3" t="n">
-        <v>0.05493072096142278</v>
+        <v>0.05493819490412082</v>
       </c>
       <c r="D3" t="n">
-        <v>0.03811961771474114</v>
+        <v>0.03812422112313504</v>
       </c>
       <c r="E3" t="n">
-        <v>0.05526329583984411</v>
+        <v>0.05527191934607805</v>
       </c>
       <c r="F3" t="n">
-        <v>0.006304163717505613</v>
+        <v>0.006305240167869668</v>
       </c>
       <c r="G3" t="n">
-        <v>0.008405551623340817</v>
+        <v>0.008406986890492889</v>
       </c>
       <c r="H3" t="n">
-        <v>0.001205758309160414</v>
+        <v>0.001205091701676568</v>
       </c>
       <c r="I3" t="n">
-        <v>0.001884889491995445</v>
+        <v>0.001884454028713176</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -5056,13 +5056,13 @@
         </is>
       </c>
       <c r="K3" t="n">
-        <v>-20.42126894313009</v>
+        <v>-20.34112652077252</v>
       </c>
       <c r="L3" t="n">
-        <v>-78.97345268455423</v>
+        <v>-78.98153005139142</v>
       </c>
       <c r="M3" t="n">
-        <v>29.27609187071208</v>
+        <v>29.32020176530945</v>
       </c>
       <c r="N3" t="n">
         <v>0.01200896</v>
@@ -5071,7 +5071,7 @@
         <v>45</v>
       </c>
       <c r="P3" t="n">
-        <v>6.028791545802179e-05</v>
+        <v>6.025458508382842e-05</v>
       </c>
       <c r="Q3" t="n">
         <v>0.0005</v>
@@ -5082,85 +5082,85 @@
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr"/>
       <c r="U3" t="n">
-        <v>0.007331939125710014</v>
+        <v>0.007330023859270633</v>
       </c>
       <c r="V3" t="n">
-        <v>0.04669145677729263</v>
+        <v>0.04669807023460655</v>
       </c>
       <c r="W3" t="n">
-        <v>0.04669145677729263</v>
+        <v>0.04669807023460655</v>
       </c>
       <c r="X3" t="n">
-        <v>0.04669145677729263</v>
+        <v>0.04669807023460655</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.03811961771474114</v>
+        <v>0.03812422112313504</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.05526329583984411</v>
+        <v>0.05527191934607805</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.05543072096142278</v>
+        <v>0.05543819490412082</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.05576329583984411</v>
+        <v>0.05577191934607805</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.05576329583984411</v>
+        <v>0.05577191934607805</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.7000125234141203</v>
+        <v>0.7000220089540585</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.6897818368490682</v>
+        <v>0.6897575038859264</v>
       </c>
       <c r="AF3" t="n">
-        <v>0.6897818368490682</v>
+        <v>0.6897575038859264</v>
       </c>
       <c r="AG3" t="n">
-        <v>0.004834323585009638</v>
+        <v>0.00483551328137777</v>
       </c>
       <c r="AH3" t="n">
-        <v>0.005029459284339527</v>
+        <v>0.005031351212977864</v>
       </c>
       <c r="AI3" t="n">
-        <v>0.0009619534952489873</v>
+        <v>0.0009616191348074418</v>
       </c>
       <c r="AJ3" t="n">
-        <v>0.01681110324668163</v>
+        <v>0.01681397378098578</v>
       </c>
       <c r="AK3" t="n">
-        <v>0.0164785283682603</v>
+        <v>0.01648024933902854</v>
       </c>
       <c r="AL3" t="n">
-        <v>0.01714367812510297</v>
+        <v>0.01714769822294301</v>
       </c>
       <c r="AM3" t="n">
-        <v>0.01714367812510297</v>
+        <v>0.01714769822294301</v>
       </c>
       <c r="AN3" t="n">
-        <v>0.04532867257218443</v>
+        <v>2.606786450047594</v>
       </c>
       <c r="AO3" t="n">
         <v>2</v>
       </c>
       <c r="AP3" t="n">
-        <v>0.75</v>
+        <v>0.7500000000000001</v>
       </c>
       <c r="AQ3" t="n">
         <v>1.333333333333333</v>
       </c>
       <c r="AR3" t="n">
-        <v>0.2242434020346054</v>
+        <v>0.2241533207152049</v>
       </c>
       <c r="AS3" t="n">
-        <v>0.0500000000000009</v>
+        <v>0.05</v>
       </c>
       <c r="AT3" t="n">
-        <v>0.0297422478860033</v>
+        <v>0.02973717019622269</v>
       </c>
       <c r="AU3" t="n">
-        <v>1.428693860692393</v>
+        <v>1.428449949598522</v>
       </c>
     </row>
   </sheetData>
@@ -5174,7 +5174,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5280,13 +5280,13 @@
         <v>52</v>
       </c>
       <c r="H3" t="n">
-        <v>-7.750284923154875</v>
+        <v>-7.750900010724145</v>
       </c>
       <c r="I3" t="n">
-        <v>1.568174037168942</v>
+        <v>1.567959843375942</v>
       </c>
       <c r="J3" t="n">
-        <v>0.6725502325756242</v>
+        <v>0.6724937636674512</v>
       </c>
     </row>
     <row r="4">
@@ -5306,13 +5306,13 @@
         <v>78</v>
       </c>
       <c r="H4" t="n">
-        <v>-9.496136858107294</v>
+        <v>-9.495427239844926</v>
       </c>
       <c r="I4" t="n">
-        <v>0.7334160347970758</v>
+        <v>0.7360460068166433</v>
       </c>
       <c r="J4" t="n">
-        <v>0.5646535678195018</v>
+        <v>0.5649333851033497</v>
       </c>
     </row>
     <row r="5">
@@ -5332,13 +5332,13 @@
         <v>104</v>
       </c>
       <c r="H5" t="n">
-        <v>-9.300573602709457</v>
+        <v>-9.299006481851682</v>
       </c>
       <c r="I5" t="n">
-        <v>0.1492775798761573</v>
+        <v>0.1492480277625871</v>
       </c>
       <c r="J5" t="n">
-        <v>0.2431598027328579</v>
+        <v>0.2434574629912753</v>
       </c>
     </row>
     <row r="6">
@@ -5358,13 +5358,13 @@
         <v>131</v>
       </c>
       <c r="H6" t="n">
-        <v>-9.892094428922363</v>
+        <v>-9.895885468843431</v>
       </c>
       <c r="I6" t="n">
-        <v>0.1477726620387331</v>
+        <v>0.1481451387670013</v>
       </c>
       <c r="J6" t="n">
-        <v>0.3503573695053961</v>
+        <v>0.3511548650367869</v>
       </c>
     </row>
     <row r="7">
@@ -5384,13 +5384,13 @@
         <v>157</v>
       </c>
       <c r="H7" t="n">
-        <v>-9.199326816237182</v>
+        <v>-9.200400345302439</v>
       </c>
       <c r="I7" t="n">
-        <v>0.03077211358777994</v>
+        <v>0.03058008668179206</v>
       </c>
       <c r="J7" t="n">
-        <v>0.3484703049592386</v>
+        <v>0.34973574484107</v>
       </c>
     </row>
     <row r="8">
@@ -5410,13 +5410,13 @@
         <v>183</v>
       </c>
       <c r="H8" t="n">
-        <v>-9.083798570756528</v>
+        <v>-9.084281500381254</v>
       </c>
       <c r="I8" t="n">
-        <v>0.00607277926910256</v>
+        <v>0.006113543923353087</v>
       </c>
       <c r="J8" t="n">
-        <v>0.1467896697841308</v>
+        <v>0.1482713070892053</v>
       </c>
     </row>
     <row r="9">
@@ -5436,13 +5436,13 @@
         <v>209</v>
       </c>
       <c r="H9" t="n">
-        <v>-9.07365649448988</v>
+        <v>-9.075120310823809</v>
       </c>
       <c r="I9" t="n">
-        <v>0.001900650217416838</v>
+        <v>0.001326394295294436</v>
       </c>
       <c r="J9" t="n">
-        <v>0.1130199865429033</v>
+        <v>0.1197777557032363</v>
       </c>
     </row>
     <row r="10">
@@ -5462,13 +5462,13 @@
         <v>235</v>
       </c>
       <c r="H10" t="n">
-        <v>-9.0878009155253</v>
+        <v>-9.08787379136759</v>
       </c>
       <c r="I10" t="n">
-        <v>0.003592890147953012</v>
+        <v>0.003356795372294247</v>
       </c>
       <c r="J10" t="n">
-        <v>0.05250650374281467</v>
+        <v>0.05692229201966011</v>
       </c>
     </row>
     <row r="11">
@@ -5488,13 +5488,13 @@
         <v>261</v>
       </c>
       <c r="H11" t="n">
-        <v>-9.081806994230675</v>
+        <v>-9.084363459139635</v>
       </c>
       <c r="I11" t="n">
-        <v>0.0009311574226521623</v>
+        <v>0.0007783550329741963</v>
       </c>
       <c r="J11" t="n">
-        <v>0.04665279620627363</v>
+        <v>0.04893035596110711</v>
       </c>
     </row>
     <row r="12">
@@ -5508,19 +5508,19 @@
         <v>11</v>
       </c>
       <c r="F12" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G12" t="n">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="H12" t="n">
-        <v>-9.09374047328113</v>
+        <v>-9.087053565403696</v>
       </c>
       <c r="I12" t="n">
-        <v>0.002360464612737839</v>
+        <v>0.001959275797268358</v>
       </c>
       <c r="J12" t="n">
-        <v>0.03672134583014187</v>
+        <v>0.04453568931513589</v>
       </c>
     </row>
     <row r="13">
@@ -5534,19 +5534,19 @@
         <v>12</v>
       </c>
       <c r="F13" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G13" t="n">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H13" t="n">
-        <v>-9.086100460928204</v>
+        <v>-9.088398835758415</v>
       </c>
       <c r="I13" t="n">
-        <v>0.002626019435303759</v>
+        <v>0.002028861003998627</v>
       </c>
       <c r="J13" t="n">
-        <v>0.05013222999870803</v>
+        <v>0.03435848350280891</v>
       </c>
     </row>
     <row r="14">
@@ -5560,19 +5560,19 @@
         <v>13</v>
       </c>
       <c r="F14" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G14" t="n">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H14" t="n">
-        <v>-9.088415479981144</v>
+        <v>-9.090085025825022</v>
       </c>
       <c r="I14" t="n">
-        <v>0.002611059278410779</v>
+        <v>0.002074208674003948</v>
       </c>
       <c r="J14" t="n">
-        <v>0.03548048781094824</v>
+        <v>0.03354657503223122</v>
       </c>
     </row>
     <row r="15">
@@ -5586,19 +5586,19 @@
         <v>14</v>
       </c>
       <c r="F15" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G15" t="n">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="H15" t="n">
-        <v>-9.0896117104227</v>
+        <v>-9.090680829093142</v>
       </c>
       <c r="I15" t="n">
-        <v>0.002555218152294498</v>
+        <v>0.002034619742846928</v>
       </c>
       <c r="J15" t="n">
-        <v>0.01560516228846782</v>
+        <v>0.009443022685586765</v>
       </c>
     </row>
     <row r="16">
@@ -5612,19 +5612,19 @@
         <v>15</v>
       </c>
       <c r="F16" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G16" t="n">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="H16" t="n">
-        <v>-9.091306797065737</v>
+        <v>-9.091307660280357</v>
       </c>
       <c r="I16" t="n">
-        <v>0.002658597735236098</v>
+        <v>0.002064209966464473</v>
       </c>
       <c r="J16" t="n">
-        <v>0.05029998028590057</v>
+        <v>0.03407629798953436</v>
       </c>
     </row>
     <row r="17">
@@ -5638,19 +5638,19 @@
         <v>16</v>
       </c>
       <c r="F17" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G17" t="n">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H17" t="n">
-        <v>-9.093270174931579</v>
+        <v>-9.096247643481824</v>
       </c>
       <c r="I17" t="n">
-        <v>0.002411296393167082</v>
+        <v>0.001335600998069067</v>
       </c>
       <c r="J17" t="n">
-        <v>0.04934055220732423</v>
+        <v>0.03972912002111297</v>
       </c>
     </row>
     <row r="18">
@@ -5664,19 +5664,19 @@
         <v>17</v>
       </c>
       <c r="F18" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G18" t="n">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="H18" t="n">
-        <v>-9.093727405339362</v>
+        <v>-9.095981075051835</v>
       </c>
       <c r="I18" t="n">
-        <v>0.002154384027057903</v>
+        <v>0.001386393842192952</v>
       </c>
       <c r="J18" t="n">
-        <v>0.02982478465504566</v>
+        <v>0.02228663744927879</v>
       </c>
     </row>
     <row r="19">
@@ -5690,19 +5690,19 @@
         <v>18</v>
       </c>
       <c r="F19" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G19" t="n">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="H19" t="n">
-        <v>-9.0941777686803</v>
+        <v>-9.095357874064451</v>
       </c>
       <c r="I19" t="n">
-        <v>0.002029266255329139</v>
+        <v>0.001462392452073945</v>
       </c>
       <c r="J19" t="n">
-        <v>0.01789641280759413</v>
+        <v>0.02317253035472832</v>
       </c>
     </row>
     <row r="20">
@@ -5716,19 +5716,19 @@
         <v>19</v>
       </c>
       <c r="F20" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G20" t="n">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="H20" t="n">
-        <v>-9.09437972757773</v>
+        <v>-9.095176934535274</v>
       </c>
       <c r="I20" t="n">
-        <v>0.002000586957496428</v>
+        <v>0.001348125078881726</v>
       </c>
       <c r="J20" t="n">
-        <v>0.005933269636395511</v>
+        <v>0.01884593589619031</v>
       </c>
     </row>
     <row r="21">
@@ -5742,19 +5742,19 @@
         <v>20</v>
       </c>
       <c r="F21" t="n">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G21" t="n">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="H21" t="n">
-        <v>-9.094456339566086</v>
+        <v>-9.095369024693216</v>
       </c>
       <c r="I21" t="n">
-        <v>0.001994782927822629</v>
+        <v>0.00128878239055628</v>
       </c>
       <c r="J21" t="n">
-        <v>0.001867133579023217</v>
+        <v>0.01466959709812831</v>
       </c>
     </row>
     <row r="22">
@@ -5768,19 +5768,19 @@
         <v>21</v>
       </c>
       <c r="F22" t="n">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G22" t="n">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="H22" t="n">
-        <v>-9.09461559535354</v>
+        <v>-9.095247366981081</v>
       </c>
       <c r="I22" t="n">
-        <v>0.001752409202213991</v>
+        <v>0.001171198047670944</v>
       </c>
       <c r="J22" t="n">
-        <v>0.0361976420112449</v>
+        <v>0.01373011227832814</v>
       </c>
     </row>
     <row r="23">
@@ -5794,19 +5794,19 @@
         <v>22</v>
       </c>
       <c r="F23" t="n">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G23" t="n">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="H23" t="n">
-        <v>-9.095223201257564</v>
+        <v>-9.094989961128956</v>
       </c>
       <c r="I23" t="n">
-        <v>0.001810167605286273</v>
+        <v>0.00109033825016024</v>
       </c>
       <c r="J23" t="n">
-        <v>0.01800564149521236</v>
+        <v>0.02190438653259699</v>
       </c>
     </row>
     <row r="24">
@@ -5820,19 +5820,19 @@
         <v>23</v>
       </c>
       <c r="F24" t="n">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G24" t="n">
-        <v>618</v>
+        <v>612</v>
       </c>
       <c r="H24" t="n">
-        <v>-9.095422879960676</v>
+        <v>-9.095647515894715</v>
       </c>
       <c r="I24" t="n">
-        <v>0.001801576485895984</v>
+        <v>0.001312971995500356</v>
       </c>
       <c r="J24" t="n">
-        <v>0.005649700398392987</v>
+        <v>0.02518670627388878</v>
       </c>
     </row>
     <row r="25">
@@ -5846,19 +5846,19 @@
         <v>24</v>
       </c>
       <c r="F25" t="n">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G25" t="n">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="H25" t="n">
-        <v>-9.095964301082853</v>
+        <v>-9.096025378492</v>
       </c>
       <c r="I25" t="n">
-        <v>0.0003304842494400162</v>
+        <v>0.001345638326062802</v>
       </c>
       <c r="J25" t="n">
-        <v>0.03568887272503663</v>
+        <v>0.01186358640700499</v>
       </c>
     </row>
     <row r="26">
@@ -5872,19 +5872,19 @@
         <v>25</v>
       </c>
       <c r="F26" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G26" t="n">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="H26" t="n">
-        <v>-9.095534059096241</v>
+        <v>-9.096190265373986</v>
       </c>
       <c r="I26" t="n">
-        <v>1.524571308422278e-05</v>
+        <v>0.001342566783113862</v>
       </c>
       <c r="J26" t="n">
-        <v>0.0106867519952686</v>
+        <v>0.004776711766525377</v>
       </c>
     </row>
     <row r="27">
@@ -5898,19 +5898,19 @@
         <v>26</v>
       </c>
       <c r="F27" t="n">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G27" t="n">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="H27" t="n">
-        <v>-9.095623354425863</v>
+        <v>-9.095821962328799</v>
       </c>
       <c r="I27" t="n">
-        <v>2.44657493458228e-05</v>
+        <v>8.80233855886231e-05</v>
       </c>
       <c r="J27" t="n">
-        <v>0.001218199048681004</v>
+        <v>0.03094392377959303</v>
       </c>
     </row>
     <row r="28">
@@ -5924,19 +5924,19 @@
         <v>27</v>
       </c>
       <c r="F28" t="n">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G28" t="n">
-        <v>726</v>
+        <v>721</v>
       </c>
       <c r="H28" t="n">
-        <v>-9.095610713411833</v>
+        <v>-9.095617767348653</v>
       </c>
       <c r="I28" t="n">
-        <v>1.26689674412872e-05</v>
+        <v>2.458042453889947e-05</v>
       </c>
       <c r="J28" t="n">
-        <v>0.002167571570079691</v>
+        <v>0.008311413515324963</v>
       </c>
     </row>
     <row r="29">
@@ -5950,19 +5950,19 @@
         <v>28</v>
       </c>
       <c r="F29" t="n">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G29" t="n">
-        <v>753</v>
+        <v>747</v>
       </c>
       <c r="H29" t="n">
-        <v>-9.095599679644216</v>
+        <v>-9.095620027148231</v>
       </c>
       <c r="I29" t="n">
-        <v>8.961206522412057e-06</v>
+        <v>7.133643385268118e-06</v>
       </c>
       <c r="J29" t="n">
-        <v>0.002690174462400978</v>
+        <v>0.005801456399371365</v>
       </c>
     </row>
     <row r="30">
@@ -5976,19 +5976,19 @@
         <v>29</v>
       </c>
       <c r="F30" t="n">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G30" t="n">
-        <v>779</v>
+        <v>774</v>
       </c>
       <c r="H30" t="n">
-        <v>-9.095579645842177</v>
+        <v>-9.095632897128965</v>
       </c>
       <c r="I30" t="n">
-        <v>1.077755106253242e-05</v>
+        <v>7.23295138604918e-06</v>
       </c>
       <c r="J30" t="n">
-        <v>0.0003961300860921275</v>
+        <v>0.001564327504673309</v>
       </c>
     </row>
     <row r="31">
@@ -6002,19 +6002,19 @@
         <v>30</v>
       </c>
       <c r="F31" t="n">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="G31" t="n">
-        <v>806</v>
+        <v>800</v>
       </c>
       <c r="H31" t="n">
-        <v>-9.095575891248327</v>
+        <v>-9.095618030869961</v>
       </c>
       <c r="I31" t="n">
-        <v>5.354093593812337e-06</v>
+        <v>3.344896351259452e-06</v>
       </c>
       <c r="J31" t="n">
-        <v>0.0006849119420880208</v>
+        <v>0.001053484836620272</v>
       </c>
     </row>
     <row r="32">
@@ -6028,19 +6028,19 @@
         <v>31</v>
       </c>
       <c r="F32" t="n">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="G32" t="n">
-        <v>835</v>
+        <v>827</v>
       </c>
       <c r="H32" t="n">
-        <v>-9.095576945257296</v>
+        <v>-9.095635621454438</v>
       </c>
       <c r="I32" t="n">
-        <v>5.169299682458717e-06</v>
+        <v>4.932336857860209e-06</v>
       </c>
       <c r="J32" t="n">
-        <v>9.240679651480234e-05</v>
+        <v>0.002120585476246674</v>
       </c>
     </row>
     <row r="33">
@@ -6054,19 +6054,19 @@
         <v>32</v>
       </c>
       <c r="F33" t="n">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="G33" t="n">
-        <v>861</v>
+        <v>854</v>
       </c>
       <c r="H33" t="n">
-        <v>-9.095575723477387</v>
+        <v>-9.095637794074438</v>
       </c>
       <c r="I33" t="n">
-        <v>5.789464350980378e-08</v>
+        <v>4.428719293361749e-06</v>
       </c>
       <c r="J33" t="n">
-        <v>0.0003263907494703921</v>
+        <v>0.001067411383924922</v>
       </c>
     </row>
     <row r="34">
@@ -6080,19 +6080,19 @@
         <v>33</v>
       </c>
       <c r="F34" t="n">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="G34" t="n">
-        <v>889</v>
+        <v>883</v>
       </c>
       <c r="H34" t="n">
-        <v>-9.095588592855574</v>
+        <v>-9.095637298473363</v>
       </c>
       <c r="I34" t="n">
-        <v>3.889674760115813e-06</v>
+        <v>4.211892342897983e-06</v>
       </c>
       <c r="J34" t="n">
-        <v>0.0002666717549334482</v>
+        <v>6.090044733390346e-05</v>
       </c>
     </row>
     <row r="35">
@@ -6103,21 +6103,47 @@
       <c r="C35" t="inlineStr"/>
       <c r="D35" t="inlineStr"/>
       <c r="E35" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F35" t="n">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="G35" t="n">
-        <v>891</v>
+        <v>909</v>
       </c>
       <c r="H35" t="n">
-        <v>-9.095588592855574</v>
+        <v>-9.095617585575955</v>
       </c>
       <c r="I35" t="n">
-        <v>3.889674760115813e-06</v>
+        <v>4.965856748029296e-07</v>
       </c>
       <c r="J35" t="n">
+        <v>0.0005034727920392823</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr"/>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" t="n">
+        <v>34</v>
+      </c>
+      <c r="F36" t="n">
+        <v>62</v>
+      </c>
+      <c r="G36" t="n">
+        <v>912</v>
+      </c>
+      <c r="H36" t="n">
+        <v>-9.095617585575955</v>
+      </c>
+      <c r="I36" t="n">
+        <v>4.965856748029296e-07</v>
+      </c>
+      <c r="J36" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update regression files for linux
</commit_message>
<xml_diff>
--- a/tests/regression_data_linux/design_optimization_linux.xlsx
+++ b/tests/regression_data_linux/design_optimization_linux.xlsx
@@ -725,7 +725,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:ED5"/>
+  <dimension ref="A1:EE5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1399,6 +1399,11 @@
           <t>blockage</t>
         </is>
       </c>
+      <c r="EE1" s="1" t="inlineStr">
+        <is>
+          <t>h_is</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -1807,6 +1812,11 @@
           <t>b''</t>
         </is>
       </c>
+      <c r="EE2" t="inlineStr">
+        <is>
+          <t>b''</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -2198,6 +2208,9 @@
       </c>
       <c r="ED3" t="n">
         <v>0</v>
+      </c>
+      <c r="EE3" t="n">
+        <v>490208.7952753123</v>
       </c>
     </row>
     <row r="4">
@@ -2575,6 +2588,7 @@
       <c r="EB4" t="inlineStr"/>
       <c r="EC4" t="inlineStr"/>
       <c r="ED4" t="inlineStr"/>
+      <c r="EE4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -2966,6 +2980,9 @@
       </c>
       <c r="ED5" t="n">
         <v>0</v>
+      </c>
+      <c r="EE5" t="n">
+        <v>474662.5556986326</v>
       </c>
     </row>
   </sheetData>
@@ -2979,7 +2996,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:ER3"/>
+  <dimension ref="A1:EN3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3690,37 +3707,17 @@
       </c>
       <c r="EL1" s="1" t="inlineStr">
         <is>
+          <t>h_is_throat</t>
+        </is>
+      </c>
+      <c r="EM1" s="1" t="inlineStr">
+        <is>
           <t>dh_s</t>
         </is>
       </c>
-      <c r="EM1" s="1" t="inlineStr">
+      <c r="EN1" s="1" t="inlineStr">
         <is>
           <t>incidence</t>
-        </is>
-      </c>
-      <c r="EN1" s="1" t="inlineStr">
-        <is>
-          <t>efficiency_drop_profile</t>
-        </is>
-      </c>
-      <c r="EO1" s="1" t="inlineStr">
-        <is>
-          <t>efficiency_drop_incidence</t>
-        </is>
-      </c>
-      <c r="EP1" s="1" t="inlineStr">
-        <is>
-          <t>efficiency_drop_secondary</t>
-        </is>
-      </c>
-      <c r="EQ1" s="1" t="inlineStr">
-        <is>
-          <t>efficiency_drop_clearance</t>
-        </is>
-      </c>
-      <c r="ER1" s="1" t="inlineStr">
-        <is>
-          <t>efficiency_drop_trailing</t>
         </is>
       </c>
     </row>
@@ -4137,25 +4134,13 @@
         <v>0</v>
       </c>
       <c r="EL2" t="n">
+        <v>490664.2221761249</v>
+      </c>
+      <c r="EM2" t="n">
         <v>445.8350650867214</v>
       </c>
-      <c r="EM2" t="n">
+      <c r="EN2" t="n">
         <v>-20.45821181387751</v>
-      </c>
-      <c r="EN2" t="n">
-        <v>0.005049283615127915</v>
-      </c>
-      <c r="EO2" t="n">
-        <v>0</v>
-      </c>
-      <c r="EP2" t="n">
-        <v>0.01070363045290857</v>
-      </c>
-      <c r="EQ2" t="n">
-        <v>0</v>
-      </c>
-      <c r="ER2" t="n">
-        <v>0.002989180947525031</v>
       </c>
     </row>
     <row r="3">
@@ -4571,25 +4556,13 @@
         <v>0</v>
       </c>
       <c r="EL3" t="n">
+        <v>478729.3881142965</v>
+      </c>
+      <c r="EM3" t="n">
         <v>985.6660745106637</v>
       </c>
-      <c r="EM3" t="n">
+      <c r="EN3" t="n">
         <v>-51.62137603518779</v>
-      </c>
-      <c r="EN3" t="n">
-        <v>0.01710710071037147</v>
-      </c>
-      <c r="EO3" t="n">
-        <v>0</v>
-      </c>
-      <c r="EP3" t="n">
-        <v>0.004717247735843015</v>
-      </c>
-      <c r="EQ3" t="n">
-        <v>0.01352764666700593</v>
-      </c>
-      <c r="ER3" t="n">
-        <v>0.006083613408287504</v>
       </c>
     </row>
   </sheetData>
@@ -4698,182 +4671,182 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
+          <t>stagger_angle</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>leading_edge_diameter</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>leading_edge_wedge_angle</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>trailing_edge_thickness</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>tip_clearance</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>throat_location_fraction</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>number_of_stages</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>number_of_cascades</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>axial_chord</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>radius_mean_in</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>radius_mean_out</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>radius_mean_throat</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>radius_hub_throat</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>radius_tip_throat</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>radius_shroud_in</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>radius_shroud_out</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>radius_shroud_throat</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>hub_tip_ratio_in</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>hub_tip_ratio_out</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>hub_tip_ratio_throat</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>A_in</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>A_out</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>A_throat</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>height</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>height_in</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>height_throat</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>height_out</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>flaring_angle</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>aspect_ratio</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>pitch_chord_ratio</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>solidity</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>maximum_thickness_chord_ratio</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>trailing_edge_thickness_opening_ratio</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>tip_clearance_height_ratio</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>leading_edge_diameter_chord_ratio</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
           <t>gauging_angle</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>stagger_angle</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>leading_edge_diameter</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>leading_edge_wedge_angle</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>trailing_edge_thickness</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>tip_clearance</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>throat_location_fraction</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>number_of_stages</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>number_of_cascades</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>axial_chord</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>radius_mean_in</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>radius_mean_out</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>radius_mean_throat</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>radius_hub_throat</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>radius_tip_throat</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>radius_shroud_in</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>radius_shroud_out</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>radius_shroud_throat</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>hub_tip_ratio_in</t>
-        </is>
-      </c>
-      <c r="AE1" s="1" t="inlineStr">
-        <is>
-          <t>hub_tip_ratio_out</t>
-        </is>
-      </c>
-      <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>hub_tip_ratio_throat</t>
-        </is>
-      </c>
-      <c r="AG1" s="1" t="inlineStr">
-        <is>
-          <t>A_in</t>
-        </is>
-      </c>
-      <c r="AH1" s="1" t="inlineStr">
-        <is>
-          <t>A_out</t>
-        </is>
-      </c>
-      <c r="AI1" s="1" t="inlineStr">
-        <is>
-          <t>A_throat</t>
-        </is>
-      </c>
-      <c r="AJ1" s="1" t="inlineStr">
-        <is>
-          <t>height</t>
-        </is>
-      </c>
-      <c r="AK1" s="1" t="inlineStr">
-        <is>
-          <t>height_in</t>
-        </is>
-      </c>
-      <c r="AL1" s="1" t="inlineStr">
-        <is>
-          <t>height_throat</t>
-        </is>
-      </c>
-      <c r="AM1" s="1" t="inlineStr">
-        <is>
-          <t>height_out</t>
-        </is>
-      </c>
-      <c r="AN1" s="1" t="inlineStr">
-        <is>
-          <t>flaring_angle</t>
-        </is>
-      </c>
-      <c r="AO1" s="1" t="inlineStr">
-        <is>
-          <t>aspect_ratio</t>
-        </is>
-      </c>
-      <c r="AP1" s="1" t="inlineStr">
-        <is>
-          <t>pitch_chord_ratio</t>
-        </is>
-      </c>
-      <c r="AQ1" s="1" t="inlineStr">
-        <is>
-          <t>solidity</t>
-        </is>
-      </c>
-      <c r="AR1" s="1" t="inlineStr">
-        <is>
-          <t>maximum_thickness_chord_ratio</t>
-        </is>
-      </c>
-      <c r="AS1" s="1" t="inlineStr">
-        <is>
-          <t>trailing_edge_thickness_opening_ratio</t>
-        </is>
-      </c>
-      <c r="AT1" s="1" t="inlineStr">
-        <is>
-          <t>tip_clearance_height_ratio</t>
-        </is>
-      </c>
-      <c r="AU1" s="1" t="inlineStr">
-        <is>
-          <t>leading_edge_diameter_chord_ratio</t>
         </is>
       </c>
     </row>
@@ -4914,34 +4887,34 @@
         <v>20.45821181387751</v>
       </c>
       <c r="L2" t="n">
-        <v>79.19999999999999</v>
+        <v>-29.37089409306124</v>
       </c>
       <c r="M2" t="n">
-        <v>-29.37089409306124</v>
+        <v>0.01200896</v>
       </c>
       <c r="N2" t="n">
-        <v>0.01200896</v>
+        <v>45</v>
       </c>
       <c r="O2" t="n">
-        <v>45</v>
+        <v>7.298183360649198e-05</v>
       </c>
       <c r="P2" t="n">
-        <v>7.298183360649198e-05</v>
+        <v>0</v>
       </c>
       <c r="Q2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R2" t="n">
         <v>1</v>
       </c>
       <c r="S2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T2" t="n">
-        <v>2</v>
+        <v>0.009051201042235821</v>
       </c>
       <c r="U2" t="n">
-        <v>0.009051201042235821</v>
+        <v>0.04669807023460655</v>
       </c>
       <c r="V2" t="n">
         <v>0.04669807023460655</v>
@@ -4950,76 +4923,76 @@
         <v>0.04669807023460655</v>
       </c>
       <c r="X2" t="n">
-        <v>0.04669807023460655</v>
+        <v>0.03845794556513049</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.03845794556513049</v>
+        <v>0.0549381949040826</v>
       </c>
       <c r="Z2" t="n">
+        <v>0.05837258779325816</v>
+      </c>
+      <c r="AA2" t="n">
         <v>0.0549381949040826</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>0.05837258779325816</v>
       </c>
       <c r="AB2" t="n">
         <v>0.0549381949040826</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.0549381949040826</v>
+        <v>0.6000000000000008</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.6000000000000008</v>
+        <v>0.700022008955241</v>
       </c>
       <c r="AE2" t="n">
         <v>0.700022008955241</v>
       </c>
       <c r="AF2" t="n">
-        <v>0.700022008955241</v>
+        <v>0.00685090177305115</v>
       </c>
       <c r="AG2" t="n">
-        <v>0.00685090177305115</v>
+        <v>0.004835513281355344</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.004835513281355344</v>
+        <v>0.0009060848353570968</v>
       </c>
       <c r="AI2" t="n">
-        <v>0.0009060848353570968</v>
+        <v>0.01991464222812767</v>
       </c>
       <c r="AJ2" t="n">
-        <v>0.01991464222812767</v>
+        <v>0.02334903511730322</v>
       </c>
       <c r="AK2" t="n">
-        <v>0.02334903511730322</v>
+        <v>0.01648024933895211</v>
       </c>
       <c r="AL2" t="n">
         <v>0.01648024933895211</v>
       </c>
       <c r="AM2" t="n">
-        <v>0.01648024933895211</v>
+        <v>-20.77877730306741</v>
       </c>
       <c r="AN2" t="n">
-        <v>-20.77877730306741</v>
+        <v>1.917411321321791</v>
       </c>
       <c r="AO2" t="n">
-        <v>1.917411321321791</v>
+        <v>0.7500000000000001</v>
       </c>
       <c r="AP2" t="n">
-        <v>0.7500000000000001</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="AQ2" t="n">
-        <v>1.333333333333333</v>
+        <v>0.2245727647673469</v>
       </c>
       <c r="AR2" t="n">
-        <v>0.2245727647673469</v>
+        <v>0.05000000000000006</v>
       </c>
       <c r="AS2" t="n">
-        <v>0.05000000000000006</v>
+        <v>0</v>
       </c>
       <c r="AT2" t="n">
-        <v>0</v>
+        <v>1.15624049870091</v>
       </c>
       <c r="AU2" t="n">
-        <v>1.15624049870091</v>
+        <v>79.19999999999999</v>
       </c>
     </row>
     <row r="3">
@@ -5059,30 +5032,30 @@
         <v>-20.34112652077252</v>
       </c>
       <c r="L3" t="n">
-        <v>-78.98153005139142</v>
+        <v>29.32020176530945</v>
       </c>
       <c r="M3" t="n">
-        <v>29.32020176530945</v>
+        <v>0.01200896</v>
       </c>
       <c r="N3" t="n">
-        <v>0.01200896</v>
+        <v>45</v>
       </c>
       <c r="O3" t="n">
-        <v>45</v>
+        <v>6.025458508382842e-05</v>
       </c>
       <c r="P3" t="n">
-        <v>6.025458508382842e-05</v>
+        <v>0.0005</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.0005</v>
-      </c>
-      <c r="R3" t="n">
         <v>1</v>
       </c>
+      <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr"/>
-      <c r="T3" t="inlineStr"/>
+      <c r="T3" t="n">
+        <v>0.007330023859270633</v>
+      </c>
       <c r="U3" t="n">
-        <v>0.007330023859270633</v>
+        <v>0.04669807023460655</v>
       </c>
       <c r="V3" t="n">
         <v>0.04669807023460655</v>
@@ -5091,76 +5064,76 @@
         <v>0.04669807023460655</v>
       </c>
       <c r="X3" t="n">
-        <v>0.04669807023460655</v>
+        <v>0.03812422112313504</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.03812422112313504</v>
+        <v>0.05527191934607805</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.05527191934607805</v>
+        <v>0.05543819490412082</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.05543819490412082</v>
+        <v>0.05577191934607805</v>
       </c>
       <c r="AB3" t="n">
         <v>0.05577191934607805</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.05577191934607805</v>
+        <v>0.7000220089540585</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.7000220089540585</v>
+        <v>0.6897575038859264</v>
       </c>
       <c r="AE3" t="n">
         <v>0.6897575038859264</v>
       </c>
       <c r="AF3" t="n">
-        <v>0.6897575038859264</v>
+        <v>0.00483551328137777</v>
       </c>
       <c r="AG3" t="n">
-        <v>0.00483551328137777</v>
+        <v>0.005031351212977864</v>
       </c>
       <c r="AH3" t="n">
-        <v>0.005031351212977864</v>
+        <v>0.0009616191348074418</v>
       </c>
       <c r="AI3" t="n">
-        <v>0.0009616191348074418</v>
+        <v>0.01681397378098578</v>
       </c>
       <c r="AJ3" t="n">
-        <v>0.01681397378098578</v>
+        <v>0.01648024933902854</v>
       </c>
       <c r="AK3" t="n">
-        <v>0.01648024933902854</v>
+        <v>0.01714769822294301</v>
       </c>
       <c r="AL3" t="n">
         <v>0.01714769822294301</v>
       </c>
       <c r="AM3" t="n">
-        <v>0.01714769822294301</v>
+        <v>2.606786450047594</v>
       </c>
       <c r="AN3" t="n">
-        <v>2.606786450047594</v>
+        <v>2</v>
       </c>
       <c r="AO3" t="n">
-        <v>2</v>
+        <v>0.7500000000000001</v>
       </c>
       <c r="AP3" t="n">
-        <v>0.7500000000000001</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="AQ3" t="n">
-        <v>1.333333333333333</v>
+        <v>0.2241533207152049</v>
       </c>
       <c r="AR3" t="n">
-        <v>0.2241533207152049</v>
+        <v>0.05</v>
       </c>
       <c r="AS3" t="n">
-        <v>0.05</v>
+        <v>0.02973717019622269</v>
       </c>
       <c r="AT3" t="n">
-        <v>0.02973717019622269</v>
+        <v>1.428449949598522</v>
       </c>
       <c r="AU3" t="n">
-        <v>1.428449949598522</v>
+        <v>-78.98153005139142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>